<commit_message>
common config for REST call host and port
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes_ff.xlsx
+++ b/apps/delphes/runtime/configuration_delphes_ff.xlsx
@@ -8,25 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48E2C33-8BEE-4727-9708-84689B18A571}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD4B1F8-B602-4792-9E46-6CD6E1068E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locale" sheetId="12" r:id="rId1"/>
-    <sheet name="frontend" sheetId="17" r:id="rId2"/>
-    <sheet name="backend" sheetId="14" r:id="rId3"/>
-    <sheet name="case_fields" sheetId="10" r:id="rId4"/>
-    <sheet name="text_analysis" sheetId="1" r:id="rId5"/>
-    <sheet name="definitions" sheetId="7" r:id="rId6"/>
-    <sheet name="intentions" sheetId="2" r:id="rId7"/>
-    <sheet name="odm" sheetId="15" r:id="rId8"/>
-    <sheet name="drools" sheetId="16" r:id="rId9"/>
-    <sheet name="email_configuration" sheetId="13" r:id="rId10"/>
-    <sheet name="email_templates" sheetId="11" r:id="rId11"/>
-    <sheet name="tests" sheetId="9" r:id="rId12"/>
-    <sheet name="tests long" sheetId="4" r:id="rId13"/>
-    <sheet name="tests short" sheetId="8" r:id="rId14"/>
+    <sheet name="common" sheetId="18" r:id="rId2"/>
+    <sheet name="frontend" sheetId="17" r:id="rId3"/>
+    <sheet name="backend" sheetId="14" r:id="rId4"/>
+    <sheet name="case_fields" sheetId="10" r:id="rId5"/>
+    <sheet name="text_analysis" sheetId="1" r:id="rId6"/>
+    <sheet name="definitions" sheetId="7" r:id="rId7"/>
+    <sheet name="intentions" sheetId="2" r:id="rId8"/>
+    <sheet name="odm" sheetId="15" r:id="rId9"/>
+    <sheet name="drools" sheetId="16" r:id="rId10"/>
+    <sheet name="email_configuration" sheetId="13" r:id="rId11"/>
+    <sheet name="email_templates" sheetId="11" r:id="rId12"/>
+    <sheet name="tests" sheetId="9" r:id="rId13"/>
+    <sheet name="tests long" sheetId="4" r:id="rId14"/>
+    <sheet name="tests short" sheetId="8" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="189">
   <si>
     <t>response_format_type</t>
   </si>
@@ -668,25 +669,28 @@
     <t>connection_to_api</t>
   </si>
   <si>
-    <t>http_connection_url</t>
-  </si>
-  <si>
-    <t>http://localhost:8002</t>
-  </si>
-  <si>
-    <t>For instance http://localhost:8002 if launched: fastapi dev .\launcher_fastapi.py --port 8002</t>
-  </si>
-  <si>
-    <t>direct</t>
-  </si>
-  <si>
     <t>Either odm, drools or the fqn of a subclass of CaseHandlingDecisionEngine,  - apps.delphes.src.app_delphes.CaseHandlingDecisionEngineDelphesPython</t>
   </si>
   <si>
-    <t>Either http or direct</t>
-  </si>
-  <si>
     <t>apps.delphes.design_time.src.app_delphes.CaseHandlingDecisionEngineDelphesPython</t>
+  </si>
+  <si>
+    <t>Either rest or direct</t>
+  </si>
+  <si>
+    <t>rest</t>
+  </si>
+  <si>
+    <t>rest_api_host</t>
+  </si>
+  <si>
+    <t>rest_api_port</t>
+  </si>
+  <si>
+    <t>127.0.0.1</t>
+  </si>
+  <si>
+    <t>locale</t>
   </si>
 </sst>
 </file>
@@ -765,7 +769,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -791,6 +795,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1092,6 +1099,41 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67526D7-3946-41B7-9C99-93B1591CF2D0}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1181,12 +1223,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1233,7 +1275,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC612E36-7152-48D2-8E3D-E1FAD4D4F885}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1278,7 +1320,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A251C2B-C886-421E-8876-0F07524CBA66}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -1467,7 +1509,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9702681-D1BC-443E-80AD-3DFE6E5250FB}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1513,17 +1555,74 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80CDFDD5-DDA9-4342-AD9F-1784F0C7F8C5}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" s="13">
+        <v>8002</v>
+      </c>
+      <c r="C4" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4770C3BF-D2D4-4BEC-BA39-094D657EDCA0}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.42578125" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="151.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1546,34 +1645,20 @@
         <v>184</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="C3" s="5" t="s">
         <v>183</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{178CE984-2701-4FB0-A6D8-D84336AB1260}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549C78AA-1218-455B-9887-3E0A5E59C6C7}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1611,10 +1696,10 @@
         <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1632,7 +1717,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
   <dimension ref="A1:J13"/>
   <sheetViews>
@@ -1993,7 +2078,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
@@ -2091,7 +2176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F212B83-BB31-486E-8D1E-C153171C389E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2158,7 +2243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
   <dimension ref="A1:C24"/>
   <sheetViews>
@@ -2420,7 +2505,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA2560B-2446-422E-A0A3-EC959CE749E5}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2464,39 +2549,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67526D7-3946-41B7-9C99-93B1591CF2D0}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>177</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Locale and localization centrally configured, client url configuration and README updated
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes_ff.xlsx
+++ b/apps/delphes/runtime/configuration_delphes_ff.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD4B1F8-B602-4792-9E46-6CD6E1068E97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F46BA102-F0AE-4096-87D5-54868A032F9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="locale" sheetId="12" r:id="rId1"/>
+    <sheet name="locale_old" sheetId="12" r:id="rId1"/>
     <sheet name="common" sheetId="18" r:id="rId2"/>
     <sheet name="frontend" sheetId="17" r:id="rId3"/>
     <sheet name="backend" sheetId="14" r:id="rId4"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="192">
   <si>
     <t>response_format_type</t>
   </si>
@@ -672,9 +672,6 @@
     <t>Either odm, drools or the fqn of a subclass of CaseHandlingDecisionEngine,  - apps.delphes.src.app_delphes.CaseHandlingDecisionEngineDelphesPython</t>
   </si>
   <si>
-    <t>apps.delphes.design_time.src.app_delphes.CaseHandlingDecisionEngineDelphesPython</t>
-  </si>
-  <si>
     <t>Either rest or direct</t>
   </si>
   <si>
@@ -691,6 +688,18 @@
   </si>
   <si>
     <t>locale</t>
+  </si>
+  <si>
+    <t>odm</t>
+  </si>
+  <si>
+    <t>http://localhost:8501</t>
+  </si>
+  <si>
+    <t>client_url</t>
+  </si>
+  <si>
+    <t>Used for defining the CORS middleware - Make sure this is the port you are using for the client</t>
   </si>
 </sst>
 </file>
@@ -1556,16 +1565,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80CDFDD5-DDA9-4342-AD9F-1784F0C7F8C5}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="86.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1581,7 +1591,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>15</v>
@@ -1590,23 +1600,37 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C3" s="5"/>
+        <v>190</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="B4" s="13">
+      <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B5" s="13">
         <v>8002</v>
       </c>
-      <c r="C4" s="5"/>
+      <c r="C5" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{3F1727BD-BDC2-475B-B4A6-D8231201080E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1642,10 +1666,10 @@
         <v>180</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1696,7 +1720,7 @@
         <v>162</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>181</v>
@@ -2083,7 +2107,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Change analyze so that it returns the list of fields specific to each intention
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes_ff.xlsx
+++ b/apps/delphes/runtime/configuration_delphes_ff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ADD4051-1EDA-4B2F-81B0-9E08FC0FFCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C88727D-B5A8-4B20-BA8F-B287C269B530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11355" yWindow="0" windowWidth="14400" windowHeight="15480" tabRatio="760" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="18" r:id="rId1"/>
@@ -692,13 +692,13 @@
     <t>Used for defining the CORS middleware - Make sure this is the port you are using for the client</t>
   </si>
   <si>
-    <t>direct</t>
-  </si>
-  <si>
     <t>Either odm, drools or the fqn of a subclass of CaseHandlingDecisionEngine,  - apps.delphes.design_time.src.app_delphes.CaseHandlingDecisionEngineDelphesPython</t>
   </si>
   <si>
     <t>http://localhost:9060/DecisionService/rest/delphes/case_handling_decision</t>
+  </si>
+  <si>
+    <t>rest</t>
   </si>
 </sst>
 </file>
@@ -1585,7 +1585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4770C3BF-D2D4-4BEC-BA39-094D657EDCA0}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1612,7 +1612,7 @@
         <v>179</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>180</v>
@@ -1669,7 +1669,7 @@
         <v>185</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2052,8 +2052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2136,7 +2136,7 @@
         <v>160</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -2502,7 +2502,7 @@
         <v>164</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add support for list of options for strings
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes_ff.xlsx
+++ b/apps/delphes/runtime/configuration_delphes_ff.xlsx
@@ -8,27 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C88727D-B5A8-4B20-BA8F-B287C269B530}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB66FBD-A98C-4149-AB60-41CF3F3268BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="18" r:id="rId1"/>
     <sheet name="frontend" sheetId="17" r:id="rId2"/>
     <sheet name="backend" sheetId="14" r:id="rId3"/>
     <sheet name="case_fields" sheetId="10" r:id="rId4"/>
-    <sheet name="text_analysis" sheetId="1" r:id="rId5"/>
-    <sheet name="definitions" sheetId="7" r:id="rId6"/>
-    <sheet name="intentions" sheetId="2" r:id="rId7"/>
-    <sheet name="odm" sheetId="15" r:id="rId8"/>
-    <sheet name="drools" sheetId="16" r:id="rId9"/>
-    <sheet name="email_configuration" sheetId="13" r:id="rId10"/>
-    <sheet name="email_templates" sheetId="11" r:id="rId11"/>
-    <sheet name="tests" sheetId="9" r:id="rId12"/>
-    <sheet name="tests long" sheetId="4" r:id="rId13"/>
-    <sheet name="tests short" sheetId="8" r:id="rId14"/>
+    <sheet name="options" sheetId="19" r:id="rId5"/>
+    <sheet name="text_analysis" sheetId="1" r:id="rId6"/>
+    <sheet name="definitions" sheetId="7" r:id="rId7"/>
+    <sheet name="intentions" sheetId="2" r:id="rId8"/>
+    <sheet name="odm" sheetId="15" r:id="rId9"/>
+    <sheet name="drools" sheetId="16" r:id="rId10"/>
+    <sheet name="email_configuration" sheetId="13" r:id="rId11"/>
+    <sheet name="email_templates" sheetId="11" r:id="rId12"/>
+    <sheet name="tests" sheetId="9" r:id="rId13"/>
+    <sheet name="tests long" sheetId="4" r:id="rId14"/>
+    <sheet name="tests short" sheetId="8" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="214">
   <si>
     <t>response_format_type</t>
   </si>
@@ -527,9 +528,6 @@
     <t>Date de la demande JJ/MM/AAAA</t>
   </si>
   <si>
-    <t>type_str</t>
-  </si>
-  <si>
     <t>Aujourd'hui est le {date_demande} (JJ/MM/AAAA).
 Vous êtes un agent en charge d'analyser des demandes en rapport avec les procédures d'Asile ou de Séjour envoyées par des demandeurs étrangers à une Préfecture de département.</t>
   </si>
@@ -698,7 +696,76 @@
     <t>http://localhost:9060/DecisionService/rest/delphes/case_handling_decision</t>
   </si>
   <si>
-    <t>rest</t>
+    <t>direct</t>
+  </si>
+  <si>
+    <t>c,d</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>a2</t>
+  </si>
+  <si>
+    <t>b2</t>
+  </si>
+  <si>
+    <t>c2</t>
+  </si>
+  <si>
+    <t>d2</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>option_ids_csv</t>
+  </si>
+  <si>
+    <t>a, b, aa</t>
+  </si>
+  <si>
+    <t>dd</t>
+  </si>
+  <si>
+    <t>test_bool</t>
+  </si>
+  <si>
+    <t>Test bool</t>
+  </si>
+  <si>
+    <t>test_str1</t>
+  </si>
+  <si>
+    <t>Test str 1</t>
+  </si>
+  <si>
+    <t>test_str2</t>
+  </si>
+  <si>
+    <t>Test str 2</t>
   </si>
 </sst>
 </file>
@@ -735,7 +802,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -745,6 +812,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -777,7 +856,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -808,6 +887,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1116,7 +1197,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>15</v>
@@ -1125,27 +1206,27 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>187</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B5" s="13">
         <v>8002</v>
@@ -1161,6 +1242,41 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67526D7-3946-41B7-9C99-93B1591CF2D0}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -1188,25 +1304,25 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>117</v>
@@ -1215,25 +1331,25 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B7" s="5">
         <v>587</v>
@@ -1250,7 +1366,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -1269,32 +1385,32 @@
         <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>175</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1302,7 +1418,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC612E36-7152-48D2-8E3D-E1FAD4D4F885}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1347,7 +1463,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A251C2B-C886-421E-8876-0F07524CBA66}">
   <dimension ref="A1:B21"/>
   <sheetViews>
@@ -1536,7 +1652,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9702681-D1BC-443E-80AD-3DFE6E5250FB}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -1585,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4770C3BF-D2D4-4BEC-BA39-094D657EDCA0}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1609,13 +1725,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -1652,32 +1768,32 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -1689,59 +1805,63 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="7" width="58" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" customWidth="1"/>
+    <col min="8" max="8" width="58" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>137</v>
+      <c r="B1" s="15" t="s">
+        <v>204</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="15" t="s">
+        <v>205</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>144</v>
-      </c>
       <c r="F1" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>124</v>
       </c>
@@ -1751,29 +1871,32 @@
       <c r="C2" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>178</v>
+      <c r="D2" s="14" t="s">
+        <v>127</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F2" s="8" t="b">
+        <v>177</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="G2" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="I2" s="7" t="s">
+      <c r="H2" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="J2" s="8" t="b">
+      <c r="K2" s="8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>125</v>
       </c>
@@ -1783,29 +1906,32 @@
       <c r="C3" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="E3" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="F3" s="8" t="b">
+      <c r="F3" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="G3" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="I3" s="7" t="s">
+      <c r="H3" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="J3" s="8" t="b">
+      <c r="K3" s="8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>115</v>
       </c>
@@ -1815,29 +1941,32 @@
       <c r="C4" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>139</v>
+      <c r="D4" s="14" t="s">
+        <v>127</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="F4" s="8" t="b">
+        <v>138</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="I4" s="7" t="s">
+      <c r="H4" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="J4" s="8" t="b">
+      <c r="K4" s="8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>113</v>
       </c>
@@ -1847,29 +1976,32 @@
       <c r="C5" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>140</v>
+      <c r="D5" s="14" t="s">
+        <v>127</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="F5" s="8" t="b">
+        <v>139</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G5" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="I5" s="7" t="s">
+      <c r="H5" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="J5" s="8" t="b">
+      <c r="K5" s="8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>117</v>
       </c>
@@ -1879,29 +2011,32 @@
       <c r="C6" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="D6" s="10" t="s">
-        <v>152</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="F6" s="8" t="b">
+      <c r="D6" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G6" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="I6" s="7" t="s">
+      <c r="H6" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J6" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="J6" s="8" t="b">
+      <c r="K6" s="8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>118</v>
       </c>
@@ -1911,29 +2046,32 @@
       <c r="C7" s="7" t="s">
         <v>119</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>158</v>
+      <c r="D7" s="14" t="s">
+        <v>127</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="F7" s="8" t="b">
+        <v>157</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G7" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="I7" s="7" t="s">
+      <c r="H7" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="J7" s="8" t="b">
+      <c r="K7" s="8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>121</v>
       </c>
@@ -1943,29 +2081,32 @@
       <c r="C8" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="F8" s="8" t="b">
+      <c r="D8" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G8" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="H8" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="I8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="J8" s="5" t="b">
+      <c r="K8" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>75</v>
       </c>
@@ -1975,73 +2116,174 @@
       <c r="C9" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="F9" s="7" t="b">
+      <c r="D9" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G9" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="7" t="s">
+      <c r="H9" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="J9" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="J9" s="8" t="b">
+      <c r="K9" s="8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G10" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="F10" s="8" t="b">
+      <c r="J10" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="K10" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="J10" s="5" t="b">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E11" s="8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="D12" t="str">
-        <f>""</f>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H13" t="str">
-        <f>""</f>
-        <v/>
+      <c r="F11" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G11" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="K11" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="K12" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="G13" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="K13" s="8" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" display="johndoe@outlook" xr:uid="{343BA063-0012-4384-B796-30762B791B20}"/>
+    <hyperlink ref="E6" r:id="rId1" display="johndoe@outlook" xr:uid="{343BA063-0012-4384-B796-30762B791B20}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2049,11 +2291,101 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6ECAA67-41A6-4458-95C4-500183FDE676}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>195</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>202</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>199</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2118,25 +2450,25 @@
         <v>111</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -2146,7 +2478,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F212B83-BB31-486E-8D1E-C153171C389E}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2213,7 +2545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
   <dimension ref="A1:C24"/>
   <sheetViews>
@@ -2475,7 +2807,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA2560B-2446-422E-A0A3-EC959CE749E5}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2499,15 +2831,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" s="7" t="b">
         <v>1</v>
@@ -2519,39 +2851,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67526D7-3946-41B7-9C99-93B1591CF2D0}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>176</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Add and manage new attrinutes of field: mandatory, help and format (for dates)
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes_ff.xlsx
+++ b/apps/delphes/runtime/configuration_delphes_ff.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB66FBD-A98C-4149-AB60-41CF3F3268BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9055138B-9FCB-4F77-9080-0626BE05E276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="frontend" sheetId="17" r:id="rId2"/>
     <sheet name="backend" sheetId="14" r:id="rId3"/>
     <sheet name="case_fields" sheetId="10" r:id="rId4"/>
-    <sheet name="options" sheetId="19" r:id="rId5"/>
+    <sheet name="id_labels" sheetId="19" r:id="rId5"/>
     <sheet name="text_analysis" sheetId="1" r:id="rId6"/>
     <sheet name="definitions" sheetId="7" r:id="rId7"/>
     <sheet name="intentions" sheetId="2" r:id="rId8"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="221">
   <si>
     <t>response_format_type</t>
   </si>
@@ -474,18 +474,12 @@
     <t>numero_AGDREF</t>
   </si>
   <si>
-    <t>Numéro AGDREF</t>
-  </si>
-  <si>
     <t>Adresse mail</t>
   </si>
   <si>
     <t>date_expiration_api</t>
   </si>
   <si>
-    <t>Date d'expiration de l'API</t>
-  </si>
-  <si>
     <t>default_value</t>
   </si>
   <si>
@@ -523,9 +517,6 @@
   </si>
   <si>
     <t>show_in_ui</t>
-  </si>
-  <si>
-    <t>Date de la demande JJ/MM/AAAA</t>
   </si>
   <si>
     <t>Aujourd'hui est le {date_demande} (JJ/MM/AAAA).
@@ -657,9 +648,6 @@
 En espérant vous avoir apporté les éléments souhaités,</t>
   </si>
   <si>
-    <t>15/9/2024</t>
-  </si>
-  <si>
     <t>connection_to_api</t>
   </si>
   <si>
@@ -741,9 +729,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>option_ids_csv</t>
-  </si>
-  <si>
     <t>a, b, aa</t>
   </si>
   <si>
@@ -766,6 +751,42 @@
   </si>
   <si>
     <t>Test str 2</t>
+  </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Date de la demande au format JJ/MM/AAAA</t>
+  </si>
+  <si>
+    <t>Date d'expiration de l'API au format JJ/MM/AAAA</t>
+  </si>
+  <si>
+    <t>allowed_values_csv</t>
+  </si>
+  <si>
+    <t>DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>15/09/2024</t>
+  </si>
+  <si>
+    <t>help_fr</t>
+  </si>
+  <si>
+    <t>mandatory</t>
+  </si>
+  <si>
+    <t>https://administration-etrangers-en-france.interieur.gouv.fr/particuliers/assets/img/form-help/numero_etranger_titre_sejour.jpg</t>
+  </si>
+  <si>
+    <t>Votre numéro Étranger</t>
+  </si>
+  <si>
+    <t>Exemple : nom@exemple.com</t>
   </si>
 </sst>
 </file>
@@ -802,7 +823,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -823,6 +844,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEE0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -856,7 +889,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -889,6 +922,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1197,7 +1232,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>15</v>
@@ -1206,27 +1241,27 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B5" s="13">
         <v>8002</v>
@@ -1265,10 +1300,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -1304,25 +1339,25 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>117</v>
@@ -1331,25 +1366,25 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B7" s="5">
         <v>587</v>
@@ -1385,32 +1420,32 @@
         <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -1725,13 +1760,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>
@@ -1768,32 +1803,32 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -1805,133 +1840,163 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.140625" customWidth="1"/>
-    <col min="8" max="8" width="58" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="45.7109375" customWidth="1"/>
+    <col min="5" max="5" width="31.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" customWidth="1"/>
+    <col min="11" max="11" width="58" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>16</v>
       </c>
       <c r="D1" s="15" t="s">
-        <v>205</v>
-      </c>
-      <c r="E1" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>209</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>213</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D2" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="J2" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="N2" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>123</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="G2" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="K2" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>125</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D3" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H3" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F3" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="G3" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="K3" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I3" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="J3" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="N3" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>115</v>
       </c>
@@ -1941,32 +2006,41 @@
       <c r="C4" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="G4" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="K4" s="8" t="b">
+      <c r="D4" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J4" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="N4" s="8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>113</v>
       </c>
@@ -1976,32 +2050,41 @@
       <c r="C5" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="D5" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="G5" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="K5" s="8" t="b">
+      <c r="D5" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J5" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="L5" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="N5" s="8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>117</v>
       </c>
@@ -2009,34 +2092,43 @@
         <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="G6" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="K6" s="8" t="b">
+        <v>119</v>
+      </c>
+      <c r="D6" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="J6" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="L6" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="M6" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="N6" s="8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>118</v>
       </c>
@@ -2044,69 +2136,87 @@
         <v>10</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="G7" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="J7" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="K7" s="8" t="b">
+        <v>219</v>
+      </c>
+      <c r="D7" s="7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E7" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J7" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="N7" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>10</v>
+        <v>120</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>210</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>127</v>
+        <v>212</v>
+      </c>
+      <c r="D8" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="G8" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H8" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J8" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="L8" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="J8" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="K8" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M8" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="N8" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>75</v>
       </c>
@@ -2114,176 +2224,221 @@
         <v>11</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>127</v>
+        <v>128</v>
+      </c>
+      <c r="D9" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="G9" s="7" t="b">
+        <v>125</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J9" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="H9" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="I9" s="7" t="s">
+      <c r="K9" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="L9" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="J9" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="K9" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M9" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="N9" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>127</v>
+        <v>164</v>
+      </c>
+      <c r="D10" s="7" t="b">
+        <v>1</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="G10" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H10" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J10" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="J10" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="K10" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="N10" s="5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="E11" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="G11" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H11" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D11" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H11" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J11" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="I11" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="K11" s="8" t="b">
+      <c r="L11" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="M11" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="N11" s="8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D12" s="7" t="s">
         <v>206</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>194</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="G12" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="K12" s="8" t="b">
+      <c r="D12" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J12" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="L12" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="M12" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="N12" s="8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>145</v>
-      </c>
-      <c r="G13" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="I13" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="K13" s="8" t="b">
+        <v>208</v>
+      </c>
+      <c r="D13" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="E13" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="J13" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="L13" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="N13" s="8" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E6" r:id="rId1" display="johndoe@outlook" xr:uid="{343BA063-0012-4384-B796-30762B791B20}"/>
+    <hyperlink ref="H6" r:id="rId1" display="johndoe@outlook" xr:uid="{343BA063-0012-4384-B796-30762B791B20}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -2292,10 +2447,13 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6ECAA67-41A6-4458-95C4-500183FDE676}">
+  <sheetPr>
+    <tabColor rgb="FFEE0000"/>
+  </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2313,66 +2471,66 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>192</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2385,7 +2543,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2450,13 +2608,13 @@
         <v>111</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B7" s="2" t="b">
         <v>1</v>
@@ -2465,7 +2623,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B8" s="2" t="b">
         <v>0</v>
@@ -2831,15 +2989,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B3" s="7" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Initiate i12n of Trusted Services and localization of Trusted Services and Delphes
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes_ff.xlsx
+++ b/apps/delphes/runtime/configuration_delphes_ff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9055138B-9FCB-4F77-9080-0626BE05E276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DF64EB-BE40-482F-801E-0573D324B00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="18" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <sheet name="tests long" sheetId="4" r:id="rId14"/>
     <sheet name="tests short" sheetId="8" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="243">
   <si>
     <t>response_format_type</t>
   </si>
@@ -88,18 +88,12 @@
     <t>bool</t>
   </si>
   <si>
-    <t># Comments must be in column A</t>
-  </si>
-  <si>
     <t>llm</t>
   </si>
   <si>
     <t>openai</t>
   </si>
   <si>
-    <t>fr</t>
-  </si>
-  <si>
     <t>label_fr</t>
   </si>
   <si>
@@ -163,9 +157,6 @@
     <t>JE VEUX RETOURNER DANS MON PAYS POUR MOTIF EXCEPTIONNEL</t>
   </si>
   <si>
-    <t>AUTRES</t>
-  </si>
-  <si>
     <t>Le document provisoire (récépissé ou API, Attestation de Prolongation d'Instruction) que le demandeur a obtenu au moment de sa demande de titre de séjour a expiré ou va bientôt expirer</t>
   </si>
   <si>
@@ -209,9 +200,6 @@
   </si>
   <si>
     <t>Le demandeur sollicite un titre vie privée et familiale hors ANEF</t>
-  </si>
-  <si>
-    <t>La demande ne correspond à aucune des intentions listées ci-dessus</t>
   </si>
   <si>
     <t>mention de risque sur l'emploi</t>
@@ -611,9 +599,6 @@
     <t>refugie_ou_protege_subsidiaire</t>
   </si>
   <si>
-    <t>Êtes-vous réfugié ou protégé subsidiaire?</t>
-  </si>
-  <si>
     <t>le demandeur est réfugié ou protégé subsidiaire</t>
   </si>
   <si>
@@ -666,9 +651,6 @@
     <t>locale</t>
   </si>
   <si>
-    <t>odm</t>
-  </si>
-  <si>
     <t>http://localhost:8501</t>
   </si>
   <si>
@@ -687,9 +669,6 @@
     <t>direct</t>
   </si>
   <si>
-    <t>c,d</t>
-  </si>
-  <si>
     <t>a</t>
   </si>
   <si>
@@ -729,30 +708,6 @@
     <t>type</t>
   </si>
   <si>
-    <t>a, b, aa</t>
-  </si>
-  <si>
-    <t>dd</t>
-  </si>
-  <si>
-    <t>test_bool</t>
-  </si>
-  <si>
-    <t>Test bool</t>
-  </si>
-  <si>
-    <t>test_str1</t>
-  </si>
-  <si>
-    <t>Test str 1</t>
-  </si>
-  <si>
-    <t>test_str2</t>
-  </si>
-  <si>
-    <t>Test str 2</t>
-  </si>
-  <si>
     <t>format</t>
   </si>
   <si>
@@ -783,10 +738,122 @@
     <t>https://administration-etrangers-en-france.interieur.gouv.fr/particuliers/assets/img/form-help/numero_etranger_titre_sejour.jpg</t>
   </si>
   <si>
-    <t>Votre numéro Étranger</t>
-  </si>
-  <si>
     <t>Exemple : nom@exemple.com</t>
+  </si>
+  <si>
+    <t>arrondissement</t>
+  </si>
+  <si>
+    <t>https://www.yvelines.gouv.fr/contenu/telechargement/29247/169330/file/bloc%201.2%20-%20Annexe%202_Liste%20des%20communes%20et%20arrondissements%201er%20janvier%202017.pdf</t>
+  </si>
+  <si>
+    <t>Versailles</t>
+  </si>
+  <si>
+    <t>Rambouillet</t>
+  </si>
+  <si>
+    <t>Saint-Germain-en-Laye</t>
+  </si>
+  <si>
+    <t>VERS</t>
+  </si>
+  <si>
+    <t>RAMB</t>
+  </si>
+  <si>
+    <t>SGEL</t>
+  </si>
+  <si>
+    <t>MLJ</t>
+  </si>
+  <si>
+    <t>Mantes-la-Jolie</t>
+  </si>
+  <si>
+    <t>VERS, RAMB, SGEL, MLJ</t>
+  </si>
+  <si>
+    <t>en</t>
+  </si>
+  <si>
+    <t>apps.delphes.design_time.src.app_delphes.CaseHandlingDecisionEngineDelphesPython</t>
+  </si>
+  <si>
+    <t>label_en</t>
+  </si>
+  <si>
+    <t>definition_en</t>
+  </si>
+  <si>
+    <t>description_en</t>
+  </si>
+  <si>
+    <t>subject_en</t>
+  </si>
+  <si>
+    <t>body_en</t>
+  </si>
+  <si>
+    <t>text_en</t>
+  </si>
+  <si>
+    <t>help_en</t>
+  </si>
+  <si>
+    <t>system_prompt_prefix_en</t>
+  </si>
+  <si>
+    <t>Today is {date_demande} (JJ/MM/AAAA).
+You are an officer responsible for reviewing applications related to asylum or residence procedures submitted by foreign applicants to a departmental prefecture in France.</t>
+  </si>
+  <si>
+    <t># Comments must be in column A before the table</t>
+  </si>
+  <si>
+    <t># Do not add a fallback intention; Such an intention called "other" will be added automatically</t>
+  </si>
+  <si>
+    <t>Le demandeur veut retourner dans son pays pour motif exceptionnel (par exemple : décès d'un proche, mariage d'un proche, naissance)</t>
+  </si>
+  <si>
+    <t>Date of application (DD/MM/YYYY)</t>
+  </si>
+  <si>
+    <t>Department of application</t>
+  </si>
+  <si>
+    <t>Surname</t>
+  </si>
+  <si>
+    <t>First name</t>
+  </si>
+  <si>
+    <t>Email address</t>
+  </si>
+  <si>
+    <t>Foreign‑national identification number (Numéro Étranger)</t>
+  </si>
+  <si>
+    <t>Numéro Étranger</t>
+  </si>
+  <si>
+    <t>District (arrondissement) of residence</t>
+  </si>
+  <si>
+    <t>API expiry date (DD/MM/YYYY)</t>
+  </si>
+  <si>
+    <t>Notice of risk on employment</t>
+  </si>
+  <si>
+    <t>Refugee status or subsidiary protection</t>
+  </si>
+  <si>
+    <t>Statut de réfugié ou protection subsidiaire</t>
+  </si>
+  <si>
+    <t>Arrondissement de rattachement de la commune de résidence</t>
   </si>
 </sst>
 </file>
@@ -889,7 +956,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -924,6 +991,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1208,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80CDFDD5-DDA9-4342-AD9F-1784F0C7F8C5}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1232,36 +1300,36 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>15</v>
+        <v>216</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="B5" s="13">
         <v>8002</v>
@@ -1300,10 +1368,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1339,52 +1407,52 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B7" s="5">
         <v>587</v>
@@ -1403,6 +1471,78 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="101" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="101" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC612E36-7152-48D2-8E3D-E1FAD4D4F885}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1411,85 +1551,42 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="101" customWidth="1"/>
+    <col min="1" max="2" width="142.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>9</v>
+        <v>223</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC612E36-7152-48D2-8E3D-E1FAD4D4F885}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="142.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>56</v>
+        <v>75</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1500,185 +1597,248 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A251C2B-C886-421E-8876-0F07524CBA66}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="142.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="142.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>99</v>
+        <v>223</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B6" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="195" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="180" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="195" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1689,41 +1849,50 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9702681-D1BC-443E-80AD-3DFE6E5250FB}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="142.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="2" width="142.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>56</v>
+        <v>75</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1760,13 +1929,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1780,7 +1949,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1803,32 +1972,32 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>180</v>
+        <v>217</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -1840,608 +2009,624 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
-  <dimension ref="A1:N13"/>
+  <sheetPr>
+    <tabColor rgb="FFEE0000"/>
+  </sheetPr>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="45.7109375" customWidth="1"/>
-    <col min="5" max="5" width="31.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="58" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="49.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="48.5703125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="13" max="13" width="58" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>202</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>196</v>
+      </c>
+      <c r="E2" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="15" t="s">
-        <v>217</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>216</v>
-      </c>
-      <c r="F1" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="D2" s="7" t="b">
+      <c r="K2" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="L2" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="J2" s="8" t="b">
+      <c r="M2" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q2" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="K2" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="M2" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="N2" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D3" s="7" t="b">
+        <v>231</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E3" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="E3" s="14" t="s">
-        <v>125</v>
-      </c>
       <c r="F3" s="14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="H3" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="L3" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="P3" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="I3" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="J3" s="8" t="b">
+      <c r="Q3" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="K3" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="L3" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="N3" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" s="7" t="b">
+        <v>232</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>125</v>
-      </c>
       <c r="F4" s="14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J4" s="8" t="b">
+        <v>121</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="L4" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="K4" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="N4" s="8" t="b">
+      <c r="M4" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="N4" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="O4" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q4" s="8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="D5" s="7" t="b">
+        <v>233</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="E5" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="E5" s="14" t="s">
-        <v>125</v>
-      </c>
       <c r="F5" s="14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J5" s="8" t="b">
+        <v>121</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I5" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="L5" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="K5" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="N5" s="8" t="b">
+      <c r="M5" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="N5" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="O5" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="P5" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q5" s="8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="D6" s="7" t="b">
+        <v>234</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="E6" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="J6" s="8" t="b">
+      <c r="F6" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="L6" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="K6" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="N6" s="8" t="b">
+      <c r="M6" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q6" s="8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>118</v>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>205</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="D7" s="7" t="b">
+        <v>237</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="E7" s="7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>206</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="L7" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q7" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J7" s="8" t="b">
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="E8" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="L8" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="K7" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="M7" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="N7" s="8" t="b">
+      <c r="M8" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q8" s="8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="D8" s="7" t="b">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="E8" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>214</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J8" s="8" t="b">
+      <c r="F9" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="K9" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="L9" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L8" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="M8" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="N8" s="5" t="b">
+      <c r="M9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="O9" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="P9" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q9" s="5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="D9" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E9" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J9" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="L9" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="N9" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>163</v>
+        <v>71</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="D10" s="7" t="b">
+        <v>239</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="E10" s="14" t="s">
-        <v>125</v>
-      </c>
       <c r="F10" s="14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J10" s="8" t="b">
+        <v>121</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="L10" s="7" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q10" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="N10" s="5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>203</v>
+        <v>159</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="D11" s="7" t="b">
+        <v>240</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="E11" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>125</v>
-      </c>
       <c r="F11" s="14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="H11" s="8" t="b">
+        <v>121</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="L11" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="I11" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J11" s="8" t="b">
+      <c r="M11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q11" s="5" t="b">
         <v>1</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="L11" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="M11" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="N11" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>205</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>206</v>
-      </c>
-      <c r="D12" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>201</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>190</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J12" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="L12" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="M12" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="N12" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>207</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>208</v>
-      </c>
-      <c r="D13" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E13" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>187</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>142</v>
-      </c>
-      <c r="J13" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="K13" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="L13" s="14" t="s">
-        <v>125</v>
-      </c>
-      <c r="M13" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="N13" s="8" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1" display="johndoe@outlook" xr:uid="{343BA063-0012-4384-B796-30762B791B20}"/>
+    <hyperlink ref="J6" r:id="rId1" display="johndoe@outlook" xr:uid="{343BA063-0012-4384-B796-30762B791B20}"/>
+    <hyperlink ref="G7" r:id="rId2" display="https://www.insee.fr/fr/metadonnees/geographie/departement/78-yvelines" xr:uid="{34439202-45B3-4546-82A4-5A474FE330D8}"/>
+    <hyperlink ref="F7" r:id="rId3" display="https://www.insee.fr/fr/metadonnees/geographie/departement/78-yvelines" xr:uid="{50A9B1EE-2F1E-46CC-9F6C-74DF4034847D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -2450,87 +2635,159 @@
   <sheetPr>
     <tabColor rgb="FFEE0000"/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>218</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C5" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>196</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>197</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>198</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>199</v>
-      </c>
       <c r="B9" s="7" t="s">
-        <v>195</v>
+        <v>188</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -2540,10 +2797,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2567,10 +2824,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>14</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -2605,30 +2862,39 @@
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>111</v>
+        <v>225</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>134</v>
+        <v>226</v>
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B7" s="2" t="b">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B8" s="2" t="b">
         <v>0</v>
       </c>
       <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2638,77 +2904,96 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F212B83-BB31-486E-8D1E-C153171C389E}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="108.28515625" customWidth="1"/>
+    <col min="2" max="3" width="108.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>219</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="C4" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B5" s="2" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="C5" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>109</v>
+      <c r="C6" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
-  <dimension ref="A1:C24"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2716,248 +3001,364 @@
     <col min="1" max="1" width="60" style="1" customWidth="1"/>
     <col min="2" max="2" width="40.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="49.7109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="40.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B5" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="C7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B6" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="B13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="B18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="B19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
+      <c r="B20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="B21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="B22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+      <c r="B23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B21" s="2" t="s">
+      <c r="B24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C24" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>53</v>
+      <c r="E24" s="2" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2989,15 +3390,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B3" s="7" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Improve test client, work on l12n
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes_ff.xlsx
+++ b/apps/delphes/runtime/configuration_delphes_ff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DF64EB-BE40-482F-801E-0573D324B00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DFB1C4-2866-474B-9195-07D3FD350907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="18" r:id="rId1"/>
@@ -25,9 +25,6 @@
     <sheet name="drools" sheetId="16" r:id="rId10"/>
     <sheet name="email_configuration" sheetId="13" r:id="rId11"/>
     <sheet name="email_templates" sheetId="11" r:id="rId12"/>
-    <sheet name="tests" sheetId="9" r:id="rId13"/>
-    <sheet name="tests long" sheetId="4" r:id="rId14"/>
-    <sheet name="tests short" sheetId="8" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="257">
   <si>
     <t>response_format_type</t>
   </si>
@@ -262,155 +259,18 @@
     <t>je_veux_retourner_dans_mon_pays_pour_motif_exceptionnel</t>
   </si>
   <si>
-    <t>autres</t>
-  </si>
-  <si>
     <t>mention_de_risque_sur_l_emploi</t>
   </si>
   <si>
     <t>date d'expiration de l'API au format JJ/MM/AAAA</t>
   </si>
   <si>
-    <t>expected_intention</t>
-  </si>
-  <si>
-    <t>[INTERNET] Deuxième convocation pour madame A A. Bonjour,  Je viens vers vous car madame A A a reçu une convocation pour prendre ses empreintes et donner ses photos d'identité mais madame A a déjà prise ses empreintes il y a un moment. Y a-t-il un problème dans son dossier ? Est-ce que madame doit venir une deuxième fois ?  
-Bien à vous </t>
-  </si>
-  <si>
-    <t>[INTERNET] Demande d'asile. Bonjour Recevez les documents pour moi Svp. Merci.</t>
-  </si>
-  <si>
-    <t>[INTERNET] 0000000003 attestation de prolongation expirée depuis le 11 octobre. Bonjour, 
-Je vous sollicite pour le compte de l'un de nos adhérents, Monsieur C C, dont le numéro de la demande de renouvellement de carte de séjour est le 7500000000000000003. En effet, l'attestation de prolongation d'instruction de Monsieur C est arrivée à expiration depuis le 11 octobre 2024. Aussi, il souhaiterait obtenir une nouvelle attestation pour pouvoir justifier de la régularité de son séjour, dans l'attente de recevoir carte de séjour. 
-Ses coordonnées: 
-Monsieur C C 78500 Sartrouville 07 00 00 00 00 CC@yahoo.com 
-Bien à vous.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[INTERNET] API + 0000000004. Bonjour,
-L’API de Mme D arrive à expiration. Pourriez-vous la renouveler s’il vous plait ?
-Je vous remercie,
-Cordialement,
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[INTERNET]E E AGDREF 0000000005. Bonjour,
-Je vous sollicite concernant l'API de Mr E E né le 00/00/0000, AGDREF 0000000005. Son attestation expire le 22/11/2024.Pouvez-vous effectuer son renouvellement s'il vous plaît ?
-Vous trouverez en PJ ses documents. 
-En vous remerciant par avance de votre retour.
-Cordialement.
-</t>
-  </si>
-  <si>
-    <t>[INTERNET] Avancement du dossier. Bonjour madame monsieur  
-Je me permets de vous contacter pour savoir de l'avancement de mon dossier numéro 7800000000000000006 Merci  Cordialement  F F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[INTERNET] DEMANDE DE RENOUVELLEMENT DE RECEPISSE N° AGDREF 0000000007 M. G G. Bonjour, 
-En tant que travailleur social, je viens auprès de vous solliciter la demande de renouvellement du récépissé de M. G G, demandeur d’asile en procédure normale, l’un de mes suivis, qui va expirer le 14.11.2024. 
-Je vous mets en pièce jointe, la copie de son récépissé qui est expiré.
-Vous souhaitant bonne réception et comptant sur votre habituelle diligence, merci. 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[INTERNET] DEMANDE DE RENOUVELLEMENT-ATDA. Bonjour Madame, Monsieur,
-Je me permets de vous écrire au sujet de l’ATDA de monsieur H H.
-Pourriez-vous lui donner un rdv ?
-Monsieur répond au numéro de téléphone suivant : 07 00 00 00 00
-N ° AGDREF : 0000000008 N° FAMILLE : 0000007
-Vous trouverez en pièce jointe une copie de l’ATDA qui expire le 23/11/2024
-Et une attestation d’hébergement.
-Vous souhaitant bonne réception,
-Cordialement.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[INTERNET] ERREUR SUR LE PRENOM. Bonjour,
-Pouvez vous corriger l'erreur sur le prénom?
-Madame s'appelle I et non I.
-Cordialement 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[INTERNET] Fwd: Fwd: DCEM demande de titre de voyage. Bonjour Madame, Monsieur, je n’arrive pas à demander un titre de voyage sur ANEF j’ai essayé dans les deux comptes de ma mère et de moi mais je n’ai pas réussi. Est-ce que je pourrais avoir un rendez-vous pour faire cela ?S’il vous plaît. Merci Cordialement 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[INTERNET] information sur procedure -M.K. AGDREF 0000000011. Bonjour
-M.K K AGDREF 0000000011 avait une convocation pour se présenter le 1 octobre 2024 a 08h30 à la préfecture du nord à Lille.
-Monsieur a bien l’intention de se présenter a ce rendez vous .
-Merci de bien vouloir lui renouveler son ATDA ce jour la car son nouveau rendez-vous à la préfecture des Yvelines est le 10/12/2024.
-Monsieur est joignable au 0700000000 qui est son nouveau numéro.
-Je reste a votre disposition pour toute autre information.
-Cordialement.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[INTERNET] Mme L L 0000000012 _ transfert 75-78. Bonjour, 
-Je me permets de vous recontacter suite au mail (joint ci-dessous) envoyé par ma collègue, courant septembre 2024, concernant le renouvellement de l’ATDA de Mme L L. 
-En effet, l’ATDA de Madame a expiré le 19/09/2024 et elle reste à ce jour sans nouvelles du renouvellement de son attestation. 
-Pourriez-vous lui transmettre une nouvelle attestation ? 
-Merci d’avance de votre retour. 
-Cordialement 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[INTERNET] M M. Bonjour,    Je vous contact de la part de Monsieur M M (numéro de la demande 0000000000000000000) AGDREF 0000000013 car Monsieur m'informe ne toujours pas avoir eu de rendez-vous à la préfecture pour poser ses empreintes. De plus Monsieur a une Attestation de Prolongation d'Instruction de la demande de titre de séjour qui expire le 14/11/2024.    Est-ce que vous pourriez lui envoyer une nouvelle Attestation, ou lui donner un rdv à la préfecture, car cela fait maintenant plus de nombreux mois que Monsieur attend ?    N'hésitez pas à revenir vers moi si vous avez besoin de plus d'informations.  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[INTERNET] rdv ou aidé pour mes démarches. bonjour puis-je reçoive ré une réponse de votre part svp jai besoin dun rdv pour faire mes papiers je suis sans activité professionnelle ni ressource jai 20 ans je vous ai répondu ya des semaines jai toujours pas de réponse venant de la préfecture jai la protection subsidiaire on me dit daller faire une demande sur ANEF ca marche pas je ne suis pas reconnu en tant quelle regarde donc donne moi une rdv directement au préfecture ca fais 2ANS que ca dure je suis sans ACTIVITÉ nom N prénom N numéro d'étranger 0000000014 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">[INTERNET] RE: 0000000015 PROBLEME ANEF. Bonjour, 
-Je reviens vers vous concernant la situation de Monsieur O O, agdref : 0000000015.
-Serait-il possible de lui donner un rendez-vous s’il vous plait ? 
-Bien cordialement, 
-</t>
-  </si>
-  <si>
-    <t>[INTERNET] RE: Blocage de titre de séjour. Bonjour, 
-Comme évoqué précédemment, cela fait un certain temps que je rencontre des difficultés pour faire la demande de titre de voyage. Malgré plusieurs tentatives avec l'ePhoto, cela ne fonctionne toujours pas. Je tiens à préciser que toutes mes informations personnelles sont correctes.
-Lors de ma dernière visite à la préfecture pour accompagner mon fils, j'ai eu l'occasion de discuter de ce problème avec l'un de vos collègues. Celui-ci m'a conseillé de vous envoyer un message afin de solliciter un rendez-vous, car il semble que ce problème ne puisse être résolu sans ma présence.
-Par conséquent, je vous saurais gré de bien vouloir accorder un rendez-vous dans les plus brefs délais pour que nous puissions résoudre ce problème.
-En espérant une réponse positive rapide de votre part,
-Cordialement</t>
-  </si>
-  <si>
-    <t>[INTERNET] Re: Bonjour, j'ai reçu un titre de séjour fin 2022. Il n'y a pas de son sur ma carte de séjour. J'aimerais savoir quel est le statut de la carte de séjour. Je vous serais très reconnaissant de m'aider, merci.. J'ai donné mes empreintes digitales, cela a pris beaucoup de temps, quel est le statut de ma carte de séjour ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[INTERNET] Re: Bonne journée, je suppose venir pour le rendez-vous aujourd'hui, mais j'ai été détenu à l'aéroport parce que je suis allé à Malte pour prendre mon rejet plus tard pour vous le présenter depuis la dernière fois que vous m'avez dit que Malte n'a pas répondu et je suis resté pendant 6 mois ..alors je montre à l'officier à l'aéroport mes documents d'asile, mon contrat de maison, mais ils disent non, ils doivent me ramener à Malte aujourd'hui, bien que j'utilise le passeport de quelqu'un pour voyager, donc c'est tout ce qui s'est passé, merci. </t>
-  </si>
-  <si>
-    <t>[INTERNET] Re: DCEM S S (0000000019). ﻿Bonjour,
-Pourriez-Vous vous générer le DCEM de ma fille S SVP? La demande était déjà traitée le 11/09/2024 et il était convenu que vous génériez le DCEM hier (jour de son RDV).
-Je vous transmets ci-joint la confirmation de la consommation du timbre + sa demande initiale.
-En vous remerciant par avance.
-Cordialement,</t>
-  </si>
-  <si>
-    <t>[INTERNET] Re: Demande de clôture de procédure Dublin - Récépissé procédure normale - T T - AGDREF 0000000020. Monsieur le Préfet,
-Je viens vers vous en ma qualité de conseil de Monsieur T T , né le 1er janvier 1998 au Darfour, Soudan, de nationalité soudanaise, 78260 Achères - AGDREF 0000000020
-Monsieur T T est entré en France et a présenté une demande de protection internationale le 20 décembre 2023. 
-Il a été placé en procédure dite « Dublin » et mis en possession d’une attestation de demande d’asile portant cette mention.
-Saisies d'une demande de prise en charge en application de l'article 13-1 du règlement (UE) n°604/2013 du 26 juin 2013, les autorités italiennes auraient donné leur accord (implicite) le 27 février 2024.Les autorités françaises disposaient donc d’un délai de six mois expirant le 27 août 2024 pour le transférer à destination de l'Italie.
-Ce délai étant expiré, je vous remercie de bien vouloir clôturer le processus de détermination de l'Etat membre responsable de l'examen de sa demande d'asile, et de convoquer Monsieur T T pour lui remettre une attestation de demande d'asile portant la mention "procédure normale" afin de lui permettre de saisir l'OFPRA.
-Dans l'attente de votre retour, je vous prie de croire, Monsieur le préfet, en l'assurance de ma considération distinguée.</t>
-  </si>
-  <si>
     <t># Does not support formulas</t>
   </si>
   <si>
-    <t>text_fr</t>
-  </si>
-  <si>
     <t>AES</t>
   </si>
   <si>
-    <t>admission exceptionnelle au séjour</t>
-  </si>
-  <si>
     <t>ANEF (Administration Numérique pour les Etrangers en France)</t>
   </si>
   <si>
@@ -420,21 +280,12 @@
     <t>API</t>
   </si>
   <si>
-    <t xml:space="preserve">Attestation de prolongation de l’instruction, document généré depuis la plateforme ANEF </t>
-  </si>
-  <si>
     <t>ATDA</t>
   </si>
   <si>
-    <t>attestation de demande d’asile</t>
-  </si>
-  <si>
     <t>DCEM</t>
   </si>
   <si>
-    <t>Document de circulation pour étranger mineur</t>
-  </si>
-  <si>
     <t>term</t>
   </si>
   <si>
@@ -505,10 +356,6 @@
   </si>
   <si>
     <t>show_in_ui</t>
-  </si>
-  <si>
-    <t>Aujourd'hui est le {date_demande} (JJ/MM/AAAA).
-Vous êtes un agent en charge d'analyser des demandes en rapport avec les procédures d'Asile ou de Séjour envoyées par des demandeurs étrangers à une Préfecture de département.</t>
   </si>
   <si>
     <t>Doe</t>
@@ -795,19 +642,12 @@
     <t>body_en</t>
   </si>
   <si>
-    <t>text_en</t>
-  </si>
-  <si>
     <t>help_en</t>
   </si>
   <si>
     <t>system_prompt_prefix_en</t>
   </si>
   <si>
-    <t>Today is {date_demande} (JJ/MM/AAAA).
-You are an officer responsible for reviewing applications related to asylum or residence procedures submitted by foreign applicants to a departmental prefecture in France.</t>
-  </si>
-  <si>
     <t># Comments must be in column A before the table</t>
   </si>
   <si>
@@ -854,6 +694,148 @@
   </si>
   <si>
     <t>Arrondissement de rattachement de la commune de résidence</t>
+  </si>
+  <si>
+    <t>Admission Exceptionnelle au Séjour</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attestation de Prolongation de l’Instruction, document généré depuis la plateforme ANEF </t>
+  </si>
+  <si>
+    <t>ATtestation de Demande d’Asile</t>
+  </si>
+  <si>
+    <t>Document de Circulation pour Etranger Mineur</t>
+  </si>
+  <si>
+    <t>Admission Exceptionnelle au Séjour (Exceptional Admission to Residence)</t>
+  </si>
+  <si>
+    <t>The platform that allows users to carry out a number of procedures: validation of a Long-Stay Visa serving as a Residence Permit, applications concerning certain residence permits, application for travel documents, application for naturalisation, application for work authorisation, and change of address</t>
+  </si>
+  <si>
+    <t>Attestation de Prolongation de l’Instruction (Certificate of Extension of Processing, a document generated from the ANEF platform)</t>
+  </si>
+  <si>
+    <t>ATtestation de Demande d’Asile (Certificate of Asylum Application)</t>
+  </si>
+  <si>
+    <t>Document de Circulation pour Etranger Mineur (Travel Document for a Minor Foreigner)</t>
+  </si>
+  <si>
+    <t>EXPIRATION OF AN API (ATTESTATION DE PROLONGATION D’INSTRUCTION – EXTENSION‑OF‑PROCESSING CERTIFICATE)</t>
+  </si>
+  <si>
+    <t>FILING AN ASYLUM APPLICATION</t>
+  </si>
+  <si>
+    <t>STATUS OF MY PENDING ASYLUM APPLICATION</t>
+  </si>
+  <si>
+    <t>EXPIRATION OF AN ATDA (ASYLUM‑SEEKER CERTIFICATE)</t>
+  </si>
+  <si>
+    <t>UPDATING ATDA INFORMATION</t>
+  </si>
+  <si>
+    <t>REQUEST CONCERNING AN ONGOING DUBLIN PROCEDURE</t>
+  </si>
+  <si>
+    <t>UKRAINIAN NATIONAL REQUESTS A NEW RESIDENCE PERMIT</t>
+  </si>
+  <si>
+    <t>UKRAINIAN NATIONAL REQUESTS RENEWAL OF THEIR PERMIT</t>
+  </si>
+  <si>
+    <t>UKRAINIAN NATIONAL – OTHER REQUEST</t>
+  </si>
+  <si>
+    <t>REQUEST FROM A STUDENT IN A MOBILITY PROGRAMME</t>
+  </si>
+  <si>
+    <t>REQUEST FROM A TRAINEE ATTACHED TO THE MEDICAL PROFESSION</t>
+  </si>
+  <si>
+    <t>DIFFICULTIES WITH THE ANEF WEBSITE</t>
+  </si>
+  <si>
+    <t>CHANGE OF STATUS FROM STUDENT TO SALARIED EMPLOYEE</t>
+  </si>
+  <si>
+    <t>CHANGE OF STATUS FROM STUDENT TO JOB SEEKER</t>
+  </si>
+  <si>
+    <t>APPLICATION FOR A “PRIVATE AND FAMILY LIFE” RESIDENCE PERMIT OUTSIDE THE ANEF PORTAL</t>
+  </si>
+  <si>
+    <t>FILING A PERMIT APPLICATION AND UNABLE TO CREATE MY ANEF ACCOUNT</t>
+  </si>
+  <si>
+    <t>FILING A PERMIT APPLICATION AND ENCOUNTERING ANOTHER BLOCKAGE ON THE ANEF SITE</t>
+  </si>
+  <si>
+    <t>FILING A PERMIT APPLICATION AND ANOTHER ANEF‑RELATED PROBLEM</t>
+  </si>
+  <si>
+    <t>I WANT TO RETURN TO MY COUNTRY FOR AN EXCEPTIONAL REASON</t>
+  </si>
+  <si>
+    <t>Expiration of your API</t>
+  </si>
+  <si>
+    <t>{prenom} {nom},
+We have processed your request dated {date_demande} regarding the expiration of an API</t>
+  </si>
+  <si>
+    <t>Your request for a safe‑conduct pass</t>
+  </si>
+  <si>
+    <t>{prenom} {nom},
+In response to your request, please send us copies of the following:
+the translated death certificate
+your birth certificate
+the date of the funeral
+your residence permit
+proof of address less than six months old, with “URGENT REQUEST FOR A SAFE-CONDUCT” in the subject line.
+I hope this gives you the information you were looking for.</t>
+  </si>
+  <si>
+    <t>DELPHES</t>
+  </si>
+  <si>
+    <t>DELPHES est une solution innovante et efficace de prétraitement et de routage intelligent des demandes adressées par des demandeurs étrangers aux préfectures. Cette solution est construite sur le framework Athena Démarches en Confiance.</t>
+  </si>
+  <si>
+    <t>app_name_fr</t>
+  </si>
+  <si>
+    <t>app_description_fr</t>
+  </si>
+  <si>
+    <t>app_name_en</t>
+  </si>
+  <si>
+    <t>app_description_en</t>
+  </si>
+  <si>
+    <t>DELPHES is an innovative, efficient solution for pre‑processing and intelligently routing applications submitted by foreign applicants to prefectural offices in France. The system is built on the Athena Trusted Services framework.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aujourd'hui est le {date_demande} (JJ/MM/AAAA).  
+Vous êtes un agent en charge d'analyser des demandes en rapport avec les procédures d'Asile ou de Séjour envoyées par des demandeurs étrangers à une Préfecture de département.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Today is {date_demande} (JJ/MM/AAAA).  
+You are an officer responsible for reviewing applications related to asylum or residence procedures submitted by foreign applicants to a departmental prefecture in France.  </t>
+  </si>
+  <si>
+    <t>Whether emails are sent or not</t>
+  </si>
+  <si>
+    <t>send_email</t>
+  </si>
+  <si>
+    <t>EXPIRATION OF AN API (EXTENSION‑OF‑PROCESSING CERTIFICATE)</t>
   </si>
 </sst>
 </file>
@@ -956,7 +938,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -992,6 +974,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1276,7 +1261,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80CDFDD5-DDA9-4342-AD9F-1784F0C7F8C5}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1300,36 +1285,36 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>176</v>
+        <v>148</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>175</v>
+        <v>147</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>177</v>
+        <v>149</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="B5" s="13">
         <v>8002</v>
@@ -1368,10 +1353,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1381,17 +1366,20 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
-  <dimension ref="A1:C7"/>
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1407,57 +1395,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>148</v>
+        <v>120</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>149</v>
+        <v>121</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>145</v>
+        <v>117</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>142</v>
+        <v>114</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>141</v>
+        <v>113</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>143</v>
+        <v>115</v>
       </c>
       <c r="B7" s="5">
         <v>587</v>
       </c>
       <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>255</v>
+      </c>
+      <c r="B8" s="5" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>254</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1474,7 +1473,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1490,414 +1489,54 @@
         <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>221</v>
+        <v>193</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>222</v>
+        <v>194</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>135</v>
+        <v>107</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>133</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>134</v>
+        <v>241</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>157</v>
+        <v>242</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>134</v>
+        <v>106</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>166</v>
+        <v>243</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>168</v>
+        <v>244</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC612E36-7152-48D2-8E3D-E1FAD4D4F885}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="142.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A251C2B-C886-421E-8876-0F07524CBA66}">
-  <dimension ref="A1:C21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="142.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="195" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9702681-D1BC-443E-80AD-3DFE6E5250FB}">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="2" width="142.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="60.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1929,13 +1568,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>180</v>
+        <v>152</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -1946,7 +1585,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549C78AA-1218-455B-9887-3E0A5E59C6C7}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -1972,34 +1611,70 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>162</v>
+        <v>249</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>245</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>178</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>155</v>
+        <v>247</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>153</v>
+        <v>245</v>
       </c>
       <c r="C4" s="5"/>
+    </row>
+    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" s="5"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2014,8 +1689,8 @@
   </sheetPr>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2041,102 +1716,102 @@
         <v>9</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>193</v>
+        <v>165</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>202</v>
+        <v>174</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>224</v>
+        <v>195</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>201</v>
+        <v>173</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>117</v>
+        <v>90</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>136</v>
+        <v>108</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>129</v>
+        <v>102</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>123</v>
+        <v>96</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="P1" s="4" t="s">
-        <v>125</v>
+        <v>98</v>
       </c>
       <c r="Q1" s="4" t="s">
-        <v>128</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>118</v>
+        <v>91</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>230</v>
+        <v>200</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="E2" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="H2" s="17" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="L2" s="8" t="b">
         <v>1</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="Q2" s="8" t="b">
         <v>1</v>
@@ -2144,52 +1819,52 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>119</v>
+        <v>92</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="E3" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>137</v>
+        <v>109</v>
       </c>
       <c r="L3" s="8" t="b">
         <v>1</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="Q3" s="8" t="b">
         <v>1</v>
@@ -2197,52 +1872,52 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>232</v>
+        <v>202</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
       <c r="E4" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>131</v>
+        <v>103</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="L4" s="8" t="b">
         <v>1</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="Q4" s="8" t="b">
         <v>0</v>
@@ -2250,52 +1925,52 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>109</v>
+        <v>82</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>233</v>
+        <v>203</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>110</v>
+        <v>83</v>
       </c>
       <c r="E5" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>132</v>
+        <v>104</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="L5" s="8" t="b">
         <v>1</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="Q5" s="8" t="b">
         <v>0</v>
@@ -2303,52 +1978,52 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>113</v>
+        <v>86</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>234</v>
+        <v>204</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>115</v>
+        <v>88</v>
       </c>
       <c r="E6" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>204</v>
+        <v>176</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>204</v>
+        <v>176</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>144</v>
+        <v>116</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="L6" s="8" t="b">
         <v>1</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="P6" s="7" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="Q6" s="8" t="b">
         <v>0</v>
@@ -2356,52 +2031,52 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>205</v>
+        <v>177</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>237</v>
+        <v>207</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>242</v>
+        <v>212</v>
       </c>
       <c r="E7" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>206</v>
+        <v>178</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>206</v>
+        <v>178</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="L7" s="8" t="b">
         <v>1</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="P7" s="7" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="Q7" s="8" t="b">
         <v>0</v>
@@ -2409,52 +2084,52 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>114</v>
+        <v>87</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="E8" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="L8" s="8" t="b">
         <v>1</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="Q8" s="8" t="b">
         <v>0</v>
@@ -2462,37 +2137,37 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>116</v>
+        <v>89</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>197</v>
+        <v>169</v>
       </c>
       <c r="E9" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="L9" s="8" t="b">
         <v>1</v>
@@ -2501,13 +2176,13 @@
         <v>51</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="Q9" s="5" t="b">
         <v>1</v>
@@ -2515,43 +2190,43 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>239</v>
+        <v>209</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>124</v>
+        <v>97</v>
       </c>
       <c r="E10" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="L10" s="7" t="b">
         <v>0</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="N10" s="7" t="s">
         <v>50</v>
@@ -2560,7 +2235,7 @@
         <v>50</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="Q10" s="8" t="b">
         <v>1</v>
@@ -2568,37 +2243,37 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>240</v>
+        <v>210</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>241</v>
+        <v>211</v>
       </c>
       <c r="E11" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>121</v>
+        <v>94</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="L11" s="8" t="b">
         <v>1</v>
@@ -2607,13 +2282,13 @@
         <v>69</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="P11" s="7" t="s">
-        <v>127</v>
+        <v>100</v>
       </c>
       <c r="Q11" s="5" t="b">
         <v>1</v>
@@ -2652,7 +2327,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>14</v>
@@ -2660,134 +2335,134 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>181</v>
+        <v>153</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>183</v>
+        <v>155</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>184</v>
+        <v>156</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>182</v>
+        <v>154</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>189</v>
+        <v>161</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>185</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>190</v>
+        <v>162</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>186</v>
+        <v>158</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>191</v>
+        <v>163</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>187</v>
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>192</v>
+        <v>164</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>188</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>207</v>
+        <v>179</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>207</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>209</v>
+        <v>181</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>209</v>
+        <v>181</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2800,7 +2475,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2862,34 +2537,34 @@
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>225</v>
+        <v>196</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>226</v>
+        <v>253</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>130</v>
+        <v>252</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="5"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="B9" s="2" t="b">
         <v>0</v>
@@ -2907,79 +2582,80 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="3" width="108.28515625" customWidth="1"/>
+    <col min="2" max="2" width="90.140625" customWidth="1"/>
+    <col min="3" max="3" width="108.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>106</v>
+        <v>79</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>108</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>97</v>
+        <v>217</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>218</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>101</v>
+        <v>219</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>101</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>103</v>
+        <v>220</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>103</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>105</v>
+        <v>221</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>105</v>
+        <v>216</v>
       </c>
     </row>
   </sheetData>
@@ -2992,8 +2668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3008,17 +2684,17 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>227</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>228</v>
+        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3026,10 +2702,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>14</v>
@@ -3043,10 +2719,10 @@
         <v>51</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>256</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>222</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
@@ -3060,10 +2736,10 @@
         <v>52</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>223</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>223</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>17</v>
@@ -3077,10 +2753,10 @@
         <v>53</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>224</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>37</v>
+        <v>224</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>18</v>
@@ -3089,15 +2765,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>225</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>38</v>
+        <v>225</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>19</v>
@@ -3111,10 +2787,10 @@
         <v>55</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>226</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>39</v>
+        <v>226</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>20</v>
@@ -3128,10 +2804,10 @@
         <v>56</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>227</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>40</v>
+        <v>227</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
@@ -3145,10 +2821,10 @@
         <v>57</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>228</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>41</v>
+        <v>228</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>22</v>
@@ -3162,10 +2838,10 @@
         <v>58</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>229</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>42</v>
+        <v>229</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>23</v>
@@ -3179,10 +2855,10 @@
         <v>59</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>24</v>
+        <v>230</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>43</v>
+        <v>230</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>24</v>
@@ -3196,10 +2872,10 @@
         <v>60</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>25</v>
+        <v>231</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>44</v>
+        <v>231</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>25</v>
@@ -3213,10 +2889,10 @@
         <v>61</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>26</v>
+        <v>232</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>45</v>
+        <v>232</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>26</v>
@@ -3230,10 +2906,10 @@
         <v>62</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>27</v>
+        <v>233</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>46</v>
+        <v>233</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>27</v>
@@ -3247,10 +2923,10 @@
         <v>63</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>28</v>
+        <v>234</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>47</v>
+        <v>234</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>28</v>
@@ -3264,10 +2940,10 @@
         <v>64</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>29</v>
+        <v>235</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>48</v>
+        <v>235</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>29</v>
@@ -3276,15 +2952,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>30</v>
+        <v>236</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>49</v>
+        <v>236</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>30</v>
@@ -3298,10 +2974,10 @@
         <v>66</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>237</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>31</v>
+        <v>237</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>31</v>
@@ -3310,15 +2986,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>67</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>32</v>
+        <v>238</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>32</v>
+        <v>238</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>32</v>
@@ -3332,10 +3008,10 @@
         <v>68</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>239</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>33</v>
+        <v>239</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>33</v>
@@ -3349,16 +3025,16 @@
         <v>69</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>34</v>
+        <v>240</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>229</v>
+        <v>240</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -3390,15 +3066,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="B3" s="7" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
Verbalization and localization of decision service out
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes_ff.xlsx
+++ b/apps/delphes/runtime/configuration_delphes_ff.xlsx
@@ -8,23 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42DFB1C4-2866-474B-9195-07D3FD350907}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E52C0373-B9CC-4EDE-8624-8EB427BA3E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="18" r:id="rId1"/>
     <sheet name="frontend" sheetId="17" r:id="rId2"/>
     <sheet name="backend" sheetId="14" r:id="rId3"/>
-    <sheet name="case_fields" sheetId="10" r:id="rId4"/>
-    <sheet name="id_labels" sheetId="19" r:id="rId5"/>
-    <sheet name="text_analysis" sheetId="1" r:id="rId6"/>
-    <sheet name="definitions" sheetId="7" r:id="rId7"/>
-    <sheet name="intentions" sheetId="2" r:id="rId8"/>
-    <sheet name="odm" sheetId="15" r:id="rId9"/>
-    <sheet name="drools" sheetId="16" r:id="rId10"/>
-    <sheet name="email_configuration" sheetId="13" r:id="rId11"/>
-    <sheet name="email_templates" sheetId="11" r:id="rId12"/>
+    <sheet name="messages_to_agent" sheetId="21" r:id="rId4"/>
+    <sheet name="messages_to_requester" sheetId="20" r:id="rId5"/>
+    <sheet name="case_fields" sheetId="10" r:id="rId6"/>
+    <sheet name="id_labels" sheetId="19" r:id="rId7"/>
+    <sheet name="text_analysis" sheetId="1" r:id="rId8"/>
+    <sheet name="definitions" sheetId="7" r:id="rId9"/>
+    <sheet name="intentions" sheetId="2" r:id="rId10"/>
+    <sheet name="odm" sheetId="15" r:id="rId11"/>
+    <sheet name="drools" sheetId="16" r:id="rId12"/>
+    <sheet name="email_configuration" sheetId="13" r:id="rId13"/>
+    <sheet name="email_templates" sheetId="11" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="280">
   <si>
     <t>response_format_type</t>
   </si>
@@ -624,9 +626,6 @@
     <t>en</t>
   </si>
   <si>
-    <t>apps.delphes.design_time.src.app_delphes.CaseHandlingDecisionEngineDelphesPython</t>
-  </si>
-  <si>
     <t>label_en</t>
   </si>
   <si>
@@ -836,6 +835,78 @@
   </si>
   <si>
     <t>EXPIRATION OF AN API (EXTENSION‑OF‑PROCESSING CERTIFICATE)</t>
+  </si>
+  <si>
+    <t>odm</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>text_en</t>
+  </si>
+  <si>
+    <t>text_fr</t>
+  </si>
+  <si>
+    <t>ACK</t>
+  </si>
+  <si>
+    <t>API_VA_EXPIRER_DANS_X_JOURS</t>
+  </si>
+  <si>
+    <t>L'API va expirer dans {0} jour(s)</t>
+  </si>
+  <si>
+    <t>API will expire in {0} day(s)</t>
+  </si>
+  <si>
+    <t>Veuillez vous adresser à votre contact OFPRA</t>
+  </si>
+  <si>
+    <t>Your request has been registered. It will be processed by an agent</t>
+  </si>
+  <si>
+    <t>Votre demande a été prise en compte. Un agent la traitera dans les plus brefs délais</t>
+  </si>
+  <si>
+    <t>Please reach out to your contact at OFPRA</t>
+  </si>
+  <si>
+    <t>CONTACT_OFPRA</t>
+  </si>
+  <si>
+    <t>VISIT_PAGE</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>Markdown link of the form [text](url)</t>
+  </si>
+  <si>
+    <t>Please visit [{0}]({1})</t>
+  </si>
+  <si>
+    <t>Veuillez consulter la page [{0}]({1})</t>
+  </si>
+  <si>
+    <t>API_EXPIREE_DEPUIS_X_JOURS</t>
+  </si>
+  <si>
+    <t>API expired {0} day(s) ago</t>
+  </si>
+  <si>
+    <t>L'API expirée sepuis {0} jour(s)</t>
+  </si>
+  <si>
+    <t>RISQUE_SUR_EMPLOI</t>
+  </si>
+  <si>
+    <t>Risk on employment</t>
+  </si>
+  <si>
+    <t>Risque sur l'emploi</t>
   </si>
 </sst>
 </file>
@@ -1330,6 +1401,430 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
+  <dimension ref="A1:E24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="60" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.7109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA2560B-2446-422E-A0A3-EC959CE749E5}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="B3" s="7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{0B2724BA-D7EB-4960-A3AF-7147620CC45E}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D67526D7-3946-41B7-9C99-93B1591CF2D0}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -1364,7 +1859,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -1449,13 +1944,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B8" s="5" t="b">
         <v>0</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -1468,7 +1963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
   <dimension ref="A1:E3"/>
   <sheetViews>
@@ -1489,10 +1984,10 @@
         <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>193</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>194</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>107</v>
@@ -1506,10 +2001,10 @@
         <v>133</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>242</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>106</v>
@@ -1523,10 +2018,10 @@
         <v>137</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>244</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>138</v>
@@ -1545,7 +2040,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1588,7 +2083,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,37 +2106,37 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>250</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>251</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -1661,7 +2156,7 @@
         <v>126</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>189</v>
+        <v>256</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>150</v>
@@ -1683,13 +2178,160 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2ED06FD-CD59-4243-896C-6A0821CD9182}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="3" max="3" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>279</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A280385-38F0-446C-9432-C0DF8BDF752B}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.85546875" customWidth="1"/>
+    <col min="3" max="3" width="73" customWidth="1"/>
+    <col min="4" max="4" width="59.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
   <sheetPr>
     <tabColor rgb="FFEE0000"/>
   </sheetPr>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -1719,7 +2361,7 @@
         <v>165</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>14</v>
@@ -1728,7 +2370,7 @@
         <v>174</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="G1" s="15" t="s">
         <v>173</v>
@@ -1752,7 +2394,7 @@
         <v>96</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>15</v>
@@ -1772,7 +2414,7 @@
         <v>167</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>168</v>
@@ -1825,7 +2467,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>93</v>
@@ -1878,7 +2520,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>85</v>
@@ -1931,7 +2573,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>83</v>
@@ -1984,7 +2626,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>88</v>
@@ -2037,10 +2679,10 @@
         <v>10</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E7" s="7" t="b">
         <v>1</v>
@@ -2090,10 +2732,10 @@
         <v>10</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>205</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>206</v>
       </c>
       <c r="E8" s="7" t="b">
         <v>0</v>
@@ -2143,7 +2785,7 @@
         <v>167</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>169</v>
@@ -2196,7 +2838,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>97</v>
@@ -2249,10 +2891,10 @@
         <v>11</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>211</v>
       </c>
       <c r="E11" s="7" t="b">
         <v>1</v>
@@ -2305,7 +2947,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6ECAA67-41A6-4458-95C4-500183FDE676}">
   <sheetPr>
     <tabColor rgb="FFEE0000"/>
@@ -2313,7 +2955,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2327,7 +2969,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>14</v>
@@ -2470,7 +3112,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -2537,10 +3179,10 @@
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -2549,7 +3191,7 @@
         <v>80</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C7" s="5"/>
     </row>
@@ -2577,12 +3219,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F212B83-BB31-486E-8D1E-C153171C389E}">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2597,7 +3239,7 @@
         <v>79</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>81</v>
@@ -2608,10 +3250,10 @@
         <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -2619,7 +3261,7 @@
         <v>74</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>75</v>
@@ -2630,10 +3272,10 @@
         <v>76</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2641,10 +3283,10 @@
         <v>77</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2652,438 +3294,14 @@
         <v>78</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
-  <dimension ref="A1:E24"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="60" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>192</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>231</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA2560B-2446-422E-A0A3-EC959CE749E5}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.5703125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="B3" s="7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{0B2724BA-D7EB-4960-A3AF-7147620CC45E}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Resolve git conflict + avoid hallucinations by searching uppercase suctring in uppercase text
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes_ff.xlsx
+++ b/apps/delphes/runtime/configuration_delphes_ff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7145334E-3E84-4198-A59C-B6DC27A8B98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86882ACD-1BE5-43BE-ACFD-174AC5C7216F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13755" yWindow="0" windowWidth="14400" windowHeight="15480" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="18" r:id="rId1"/>
@@ -718,9 +718,6 @@
     <t>DELPHES</t>
   </si>
   <si>
-    <t>DELPHES est une solution innovante et efficace de prétraitement et de routage intelligent des demandes adressées par des demandeurs étrangers aux préfectures. Cette solution est construite sur le framework Athena Démarches en Confiance.</t>
-  </si>
-  <si>
     <t>app_name_fr</t>
   </si>
   <si>
@@ -888,7 +885,11 @@
     <t>depot_dem_titre_autre_blocage_anef</t>
   </si>
   <si>
-    <t>Demandeurs Etrangers : Logique de Priorisation et Hiérarchisation des E-mails pour les Services  
+    <t>Demandeurs Etrangers, Logique de Priorisation et Hiérarchisation des E-mails pour les Services  
+DELPHES est une solution innovante et efficace de prétraitement et de routage intelligent des demandes adressées par des demandeurs étrangers aux préfectures. Cette solution est construite sur le framework Athena Démarches en Confiance.</t>
+  </si>
+  <si>
+    <t>Demandeurs Etrangers, Logique de Priorisation et Hiérarchisation des E-mails pour les Services  
 DELPHES is an innovative, efficient solution for pre‑processing and intelligently routing applications submitted by foreign applicants to prefectural offices in France. The system is built on the Athena Trusted Services framework.</t>
   </si>
 </sst>
@@ -1387,8 +1388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1438,7 +1439,7 @@
         <v>51</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>193</v>
@@ -1477,7 +1478,7 @@
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>195</v>
@@ -1540,7 +1541,7 @@
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>198</v>
@@ -1561,7 +1562,7 @@
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>199</v>
@@ -1582,7 +1583,7 @@
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>200</v>
@@ -1603,7 +1604,7 @@
     </row>
     <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>201</v>
@@ -1624,7 +1625,7 @@
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>202</v>
@@ -1645,7 +1646,7 @@
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>203</v>
@@ -1666,7 +1667,7 @@
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>204</v>
@@ -1687,7 +1688,7 @@
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>205</v>
@@ -1708,7 +1709,7 @@
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>206</v>
@@ -1729,7 +1730,7 @@
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>207</v>
@@ -1750,7 +1751,7 @@
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>208</v>
@@ -1771,7 +1772,7 @@
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>209</v>
@@ -1792,7 +1793,7 @@
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>210</v>
@@ -1813,7 +1814,7 @@
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>211</v>
@@ -2009,13 +2010,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B8" s="5" t="b">
         <v>0</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2147,8 +2148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549C78AA-1218-455B-9887-3E0A5E59C6C7}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2171,7 +2172,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>216</v>
@@ -2180,7 +2181,7 @@
     </row>
     <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>273</v>
@@ -2189,19 +2190,19 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>216</v>
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>217</v>
+        <v>272</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -2221,7 +2222,7 @@
         <v>111</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>135</v>
@@ -2260,46 +2261,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>227</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>232</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>247</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>248</v>
       </c>
     </row>
   </sheetData>
@@ -2328,53 +2329,53 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>228</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>234</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>235</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>242</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -2396,8 +2397,8 @@
   </sheetPr>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2884,7 +2885,7 @@
         <v>51</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>56</v>
@@ -2937,7 +2938,7 @@
         <v>79</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="O10" s="7" t="s">
         <v>50</v>
@@ -2987,10 +2988,10 @@
         <v>1</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>117</v>
@@ -3157,13 +3158,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>270</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -3171,7 +3172,7 @@
         <v>168</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C7" s="5"/>
     </row>
@@ -3180,7 +3181,7 @@
         <v>65</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -3272,7 +3273,7 @@
         <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>187</v>

</xml_diff>

<commit_message>
Update Python Decision Engine
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes_ff.xlsx
+++ b/apps/delphes/runtime/configuration_delphes_ff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86882ACD-1BE5-43BE-ACFD-174AC5C7216F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA23D501-1DC6-4CAD-B8A7-6F0817844054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13755" yWindow="0" windowWidth="14400" windowHeight="15480" tabRatio="760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="18" r:id="rId1"/>
@@ -464,9 +464,6 @@
     <t>Used for defining the CORS middleware - Make sure this is the port you are using for the client</t>
   </si>
   <si>
-    <t>Either odm, drools or the fqn of a subclass of CaseHandlingDecisionEngine,  - apps.delphes.design_time.src.app_delphes.CaseHandlingDecisionEngineDelphesPython</t>
-  </si>
-  <si>
     <t>http://localhost:9060/DecisionService/rest/delphes/case_handling_decision</t>
   </si>
   <si>
@@ -739,9 +736,6 @@
     <t>EXPIRATION OF AN API (EXTENSION‑OF‑PROCESSING CERTIFICATE)</t>
   </si>
   <si>
-    <t>odm</t>
-  </si>
-  <si>
     <t>key</t>
   </si>
   <si>
@@ -891,6 +885,12 @@
   <si>
     <t>Demandeurs Etrangers, Logique de Priorisation et Hiérarchisation des E-mails pour les Services  
 DELPHES is an innovative, efficient solution for pre‑processing and intelligently routing applications submitted by foreign applicants to prefectural offices in France. The system is built on the Athena Trusted Services framework.</t>
+  </si>
+  <si>
+    <t>apps.delphes.design_time.src.decision_engine_delphes_python.CaseHandlingDecisionEngineDelphesPython</t>
+  </si>
+  <si>
+    <t>Either odm, drools or the fqn of a subclass of CaseHandlingDecisionEngine,  as: apps.delphes.design_time.src.decision_engine_delphes_python.CaseHandlingDecisionEngineDelphesPython</t>
   </si>
 </sst>
 </file>
@@ -1343,7 +1343,7 @@
         <v>131</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -1404,12 +1404,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1422,10 +1422,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>14</v>
@@ -1439,10 +1439,10 @@
         <v>51</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
@@ -1460,10 +1460,10 @@
         <v>52</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>17</v>
@@ -1478,13 +1478,13 @@
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>18</v>
@@ -1502,10 +1502,10 @@
         <v>53</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>19</v>
@@ -1523,10 +1523,10 @@
         <v>54</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>20</v>
@@ -1541,13 +1541,13 @@
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
@@ -1562,13 +1562,13 @@
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>22</v>
@@ -1583,13 +1583,13 @@
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>23</v>
@@ -1604,13 +1604,13 @@
     </row>
     <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>24</v>
@@ -1625,13 +1625,13 @@
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>25</v>
@@ -1646,13 +1646,13 @@
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>26</v>
@@ -1667,13 +1667,13 @@
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>27</v>
@@ -1688,13 +1688,13 @@
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>28</v>
@@ -1709,13 +1709,13 @@
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>29</v>
@@ -1730,13 +1730,13 @@
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>30</v>
@@ -1751,13 +1751,13 @@
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>31</v>
@@ -1772,13 +1772,13 @@
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>32</v>
@@ -1793,13 +1793,13 @@
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>33</v>
@@ -1814,19 +1814,19 @@
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
@@ -1871,7 +1871,7 @@
         <v>113</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2010,13 +2010,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B8" s="5" t="b">
         <v>0</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -2034,7 +2034,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2050,10 +2050,10 @@
         <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>166</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>92</v>
@@ -2067,10 +2067,10 @@
         <v>118</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>213</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>91</v>
@@ -2084,10 +2084,10 @@
         <v>122</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>123</v>
@@ -2132,7 +2132,7 @@
         <v>126</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>127</v>
@@ -2148,8 +2148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549C78AA-1218-455B-9887-3E0A5E59C6C7}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2172,37 +2172,37 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -2222,10 +2222,10 @@
         <v>111</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>224</v>
+        <v>272</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>135</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2261,46 +2261,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>225</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>231</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>245</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2329,53 +2329,53 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>227</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -2397,8 +2397,8 @@
   </sheetPr>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2425,28 +2425,28 @@
         <v>9</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H1" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I1" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>75</v>
@@ -2461,7 +2461,7 @@
         <v>81</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>15</v>
@@ -2478,13 +2478,13 @@
         <v>76</v>
       </c>
       <c r="B2" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>140</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>172</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>141</v>
       </c>
       <c r="E2" s="7" t="b">
         <v>1</v>
@@ -2496,13 +2496,13 @@
         <v>79</v>
       </c>
       <c r="H2" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>144</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>145</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>94</v>
@@ -2534,7 +2534,7 @@
         <v>10</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>78</v>
@@ -2587,7 +2587,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>70</v>
@@ -2640,7 +2640,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>68</v>
@@ -2693,7 +2693,7 @@
         <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>73</v>
@@ -2702,10 +2702,10 @@
         <v>1</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H6" s="14" t="s">
         <v>79</v>
@@ -2740,34 +2740,34 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E7" s="7" t="b">
         <v>1</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G7" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H7" s="14" t="s">
         <v>79</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K7" s="11" t="s">
         <v>95</v>
@@ -2799,19 +2799,19 @@
         <v>10</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>177</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>178</v>
       </c>
       <c r="E8" s="7" t="b">
         <v>0</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H8" s="14" t="s">
         <v>79</v>
@@ -2849,13 +2849,13 @@
         <v>74</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E9" s="7" t="b">
         <v>1</v>
@@ -2867,7 +2867,7 @@
         <v>79</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I9" s="14" t="s">
         <v>79</v>
@@ -2885,7 +2885,7 @@
         <v>51</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>56</v>
@@ -2905,7 +2905,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>82</v>
@@ -2938,7 +2938,7 @@
         <v>79</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="O10" s="7" t="s">
         <v>50</v>
@@ -2958,10 +2958,10 @@
         <v>11</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>182</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>183</v>
       </c>
       <c r="E11" s="7" t="b">
         <v>1</v>
@@ -2988,10 +2988,10 @@
         <v>1</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>117</v>
@@ -3036,7 +3036,7 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>14</v>
@@ -3044,46 +3044,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>158</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>159</v>
-      </c>
       <c r="C5" s="7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -3095,8 +3095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3158,21 +3158,21 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>268</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C7" s="5"/>
     </row>
@@ -3181,7 +3181,7 @@
         <v>65</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -3199,7 +3199,7 @@
         <v>109</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="5"/>
     </row>
@@ -3229,7 +3229,7 @@
         <v>64</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>66</v>
@@ -3240,10 +3240,10 @@
         <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -3251,7 +3251,7 @@
         <v>59</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>60</v>
@@ -3262,10 +3262,10 @@
         <v>61</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3273,10 +3273,10 @@
         <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3284,10 +3284,10 @@
         <v>63</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Read sample_text from configuration
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes_ff.xlsx
+++ b/apps/delphes/runtime/configuration_delphes_ff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA23D501-1DC6-4CAD-B8A7-6F0817844054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F8662A-EA97-480A-9539-A87A1C5E913B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="18" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="287">
   <si>
     <t>response_format_type</t>
   </si>
@@ -891,6 +891,59 @@
   </si>
   <si>
     <t>Either odm, drools or the fqn of a subclass of CaseHandlingDecisionEngine,  as: apps.delphes.design_time.src.decision_engine_delphes_python.CaseHandlingDecisionEngineDelphesPython</t>
+  </si>
+  <si>
+    <t>sample_text_en</t>
+  </si>
+  <si>
+    <t>sample_text_fr</t>
+  </si>
+  <si>
+    <t>Bonjour, 
+Je vous sollicite pour le compte de l'un de nos adhérents, Monsieur C C, dont la situation est assez complexe, et dont le numéro de la demande de renouvellement de carte de séjour est le 7500000000000000003.
+Il bénéficie actuellement du statut de protection subsidiaire et aimerait se rendre dans son pays de façon temporaire et exceptionnelle pour assister aux obsèques de son père.
+Il aimerait déposer une demande de droit d'asile.
+Par ailleurs, l'attestation de prolongation d'instruction de Monsieur C est arrivée à expiration depuis le 11 octobre 2024. Aussi, il souhaiterait obtenir une nouvelle attestation pour pouvoir justifier de la régularité de son séjour, dans l'attente de recevoir carte de séjour. 
+Sans action dans les prochains jours, il risquera de perdre son travail.
+Je vous remercie par avance et vous prie de noter l'urgence. Il risque son emploi, c'est donc très important.
+Monsieur C aimerait, par ailleurs, faire une demande d'Asile à la France.</t>
+  </si>
+  <si>
+    <t>Hello,
+I am writing on behalf of one of our members, Mr C C, whose case is rather complex and whose residence‑permit renewal application number (numéro de la demande de renouvellement de carte de séjour) is 7500000000000000003.
+He currently holds subsidiary protection status and would like to travel to his home country, on a temporary and exceptional basis, to attend his father’s funeral.
+He would also like to submit an asylum application.
+In addition, Mr C’s processing‑extension certificate expired on 11 October 2024. He therefore wishes to obtain a new certificate so he can prove the legality of his stay while awaiting his residence permit.
+Without action in the next few days, he risks losing his job.
+Thank you in advance for your attention; please note the urgency—his employment is at stake, so this matter is very important.
+Mr C would furthermore like to file an asylum request with France.</t>
+  </si>
+  <si>
+    <t>{departement} == 78</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>ANT</t>
+  </si>
+  <si>
+    <t>Antony</t>
+  </si>
+  <si>
+    <t>BOULO</t>
+  </si>
+  <si>
+    <t>Boulogne-Billancourt</t>
+  </si>
+  <si>
+    <t>NANTER</t>
+  </si>
+  <si>
+    <t>Nanterre</t>
+  </si>
+  <si>
+    <t>{departement} == 92</t>
   </si>
 </sst>
 </file>
@@ -2103,16 +2156,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4770C3BF-D2D4-4BEC-BA39-094D657EDCA0}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1"/>
-    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="148.85546875" customWidth="1"/>
     <col min="3" max="3" width="151.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2137,6 +2190,24 @@
       <c r="C2" s="2" t="s">
         <v>127</v>
       </c>
+    </row>
+    <row r="3" spans="1:3" ht="255" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" ht="270" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="C4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2149,7 +2220,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2398,7 +2469,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3019,19 +3090,20 @@
   <sheetPr>
     <tabColor rgb="FFEE0000"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3041,8 +3113,11 @@
       <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>154</v>
       </c>
@@ -3052,8 +3127,11 @@
       <c r="C2" s="7" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>155</v>
       </c>
@@ -3063,8 +3141,11 @@
       <c r="C3" s="7" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>156</v>
       </c>
@@ -3074,8 +3155,11 @@
       <c r="C4" s="7" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>157</v>
       </c>
@@ -3084,6 +3168,51 @@
       </c>
       <c r="C5" s="7" t="s">
         <v>158</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -3095,8 +3224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3190,7 +3319,7 @@
         <v>108</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="5"/>
     </row>

</xml_diff>

<commit_message>
Add predef config columns in tab text_analysis
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes_ff.xlsx
+++ b/apps/delphes/runtime/configuration_delphes_ff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F8662A-EA97-480A-9539-A87A1C5E913B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC110103-2244-4C92-883F-1139CF8F541E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="973" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="18" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="295">
   <si>
     <t>response_format_type</t>
   </si>
@@ -536,9 +536,6 @@
     <t>Mantes-la-Jolie</t>
   </si>
   <si>
-    <t>VERS, RAMB, SGEL, MLJ</t>
-  </si>
-  <si>
     <t>en</t>
   </si>
   <si>
@@ -922,9 +919,6 @@
     <t>{departement} == 78</t>
   </si>
   <si>
-    <t>Condition</t>
-  </si>
-  <si>
     <t>ANT</t>
   </si>
   <si>
@@ -944,6 +938,36 @@
   </si>
   <si>
     <t>{departement} == 92</t>
+  </si>
+  <si>
+    <t>condition</t>
+  </si>
+  <si>
+    <t>VERS, RAMB, SGEL, MLJ, ANT, BOULO, NANTER, TOTO</t>
+  </si>
+  <si>
+    <t>openai, ollama or scaleway</t>
+  </si>
+  <si>
+    <t>Ready to copy-paste values</t>
+  </si>
+  <si>
+    <t>ollama</t>
+  </si>
+  <si>
+    <t>scaleway</t>
+  </si>
+  <si>
+    <t>gpt-4o-mini, mistral-small or mistral-small-3.1-24b-instruct-2503</t>
+  </si>
+  <si>
+    <t>mistral-small</t>
+  </si>
+  <si>
+    <t>mistral-small-3.1-24b-instruct-2503</t>
+  </si>
+  <si>
+    <t>json_object</t>
   </si>
 </sst>
 </file>
@@ -980,7 +1004,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1001,12 +1025,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEE0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1046,7 +1064,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1078,11 +1096,16 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1396,7 +1419,7 @@
         <v>131</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -1457,12 +1480,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1475,10 +1498,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>14</v>
@@ -1492,10 +1515,10 @@
         <v>51</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
@@ -1513,10 +1536,10 @@
         <v>52</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>17</v>
@@ -1531,13 +1554,13 @@
     </row>
     <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>18</v>
@@ -1555,10 +1578,10 @@
         <v>53</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>19</v>
@@ -1576,10 +1599,10 @@
         <v>54</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>20</v>
@@ -1594,13 +1617,13 @@
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
@@ -1615,13 +1638,13 @@
     </row>
     <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>22</v>
@@ -1636,13 +1659,13 @@
     </row>
     <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>23</v>
@@ -1657,13 +1680,13 @@
     </row>
     <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>24</v>
@@ -1678,13 +1701,13 @@
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>25</v>
@@ -1699,13 +1722,13 @@
     </row>
     <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>26</v>
@@ -1720,13 +1743,13 @@
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>27</v>
@@ -1741,13 +1764,13 @@
     </row>
     <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>28</v>
@@ -1762,13 +1785,13 @@
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>29</v>
@@ -1783,13 +1806,13 @@
     </row>
     <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>30</v>
@@ -1804,13 +1827,13 @@
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>31</v>
@@ -1825,13 +1848,13 @@
     </row>
     <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>32</v>
@@ -1846,13 +1869,13 @@
     </row>
     <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>33</v>
@@ -1867,19 +1890,19 @@
     </row>
     <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="F24" s="1">
         <f t="shared" si="0"/>
@@ -1980,9 +2003,6 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2062,14 +2082,14 @@
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
-        <v>221</v>
+      <c r="A8" s="17" t="s">
+        <v>220</v>
       </c>
       <c r="B8" s="5" t="b">
         <v>0</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
   </sheetData>
@@ -2087,7 +2107,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2103,10 +2123,10 @@
         <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>164</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>92</v>
@@ -2120,10 +2140,10 @@
         <v>118</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>91</v>
@@ -2137,10 +2157,10 @@
         <v>122</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>213</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>214</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>123</v>
@@ -2158,7 +2178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4770C3BF-D2D4-4BEC-BA39-094D657EDCA0}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -2193,19 +2213,19 @@
     </row>
     <row r="3" spans="1:3" ht="255" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="270" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>274</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>275</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>276</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -2243,37 +2263,37 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -2293,10 +2313,10 @@
         <v>111</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2316,9 +2336,6 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2ED06FD-CD59-4243-896C-6A0821CD9182}">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2332,46 +2349,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>227</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>229</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>241</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>244</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -2381,9 +2398,6 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A280385-38F0-446C-9432-C0DF8BDF752B}">
-  <sheetPr>
-    <tabColor rgb="FFFF0000"/>
-  </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2400,53 +2414,53 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>222</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>225</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>231</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>232</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>239</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -2463,13 +2477,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
-  <sheetPr>
-    <tabColor rgb="FFEE0000"/>
-  </sheetPr>
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2480,7 +2491,7 @@
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="48.5703125" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.140625" customWidth="1"/>
     <col min="12" max="12" width="11.140625" customWidth="1"/>
@@ -2495,28 +2506,28 @@
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="4" t="s">
         <v>137</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="F1" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="4" t="s">
         <v>142</v>
       </c>
       <c r="J1" s="4" t="s">
@@ -2532,7 +2543,7 @@
         <v>81</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>15</v>
@@ -2545,14 +2556,14 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="18" t="s">
         <v>139</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>140</v>
@@ -2566,7 +2577,7 @@
       <c r="G2" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="15" t="s">
         <v>143</v>
       </c>
       <c r="I2" s="14" t="s">
@@ -2598,14 +2609,14 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>78</v>
@@ -2651,14 +2662,14 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>70</v>
@@ -2704,14 +2715,14 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>68</v>
@@ -2757,14 +2768,14 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>73</v>
@@ -2810,32 +2821,32 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="18" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E7" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="F7" s="18" t="s">
+      <c r="F7" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="16" t="s">
         <v>150</v>
       </c>
       <c r="H7" s="14" t="s">
         <v>79</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>159</v>
+        <v>286</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>154</v>
@@ -2863,25 +2874,25 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="18" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>177</v>
       </c>
       <c r="E8" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="F8" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="15" t="s">
         <v>147</v>
       </c>
       <c r="H8" s="14" t="s">
@@ -2916,14 +2927,14 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="18" t="s">
         <v>139</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>141</v>
@@ -2937,7 +2948,7 @@
       <c r="G9" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="15" t="s">
         <v>143</v>
       </c>
       <c r="I9" s="14" t="s">
@@ -2956,7 +2967,7 @@
         <v>51</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>56</v>
@@ -2969,14 +2980,14 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>82</v>
@@ -3009,7 +3020,7 @@
         <v>79</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="O10" s="7" t="s">
         <v>50</v>
@@ -3022,17 +3033,17 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="18" t="s">
         <v>116</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="18" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>181</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>182</v>
       </c>
       <c r="E11" s="7" t="b">
         <v>1</v>
@@ -3059,10 +3070,10 @@
         <v>1</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>117</v>
@@ -3087,13 +3098,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6ECAA67-41A6-4458-95C4-500183FDE676}">
-  <sheetPr>
-    <tabColor rgb="FFEE0000"/>
-  </sheetPr>
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3108,13 +3116,13 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3128,7 +3136,7 @@
         <v>151</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -3142,7 +3150,7 @@
         <v>152</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -3156,7 +3164,7 @@
         <v>153</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3170,49 +3178,49 @@
         <v>158</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>284</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>285</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -3222,21 +3230,24 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="86.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="28.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="59.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
@@ -3246,26 +3257,77 @@
       <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="19" t="s">
+        <v>288</v>
+      </c>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="5" t="s">
+        <v>291</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -3275,46 +3337,113 @@
       <c r="C4" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B6" s="5">
         <v>1</v>
       </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>266</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>267</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+    </row>
+    <row r="7" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+    </row>
+    <row r="8" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>65</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>108</v>
       </c>
@@ -3322,8 +3451,19 @@
         <v>1</v>
       </c>
       <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>109</v>
       </c>
@@ -3331,8 +3471,22 @@
         <v>1</v>
       </c>
       <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:N1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3358,7 +3512,7 @@
         <v>64</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>66</v>
@@ -3369,10 +3523,10 @@
         <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -3380,7 +3534,7 @@
         <v>59</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>60</v>
@@ -3391,10 +3545,10 @@
         <v>61</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3402,10 +3556,10 @@
         <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3413,10 +3567,10 @@
         <v>63</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Support dynamic lists in Trusted Services such list of arrondissements in Delples
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes_ff.xlsx
+++ b/apps/delphes/runtime/configuration_delphes_ff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC110103-2244-4C92-883F-1139CF8F541E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EACC30-1621-4C02-9A1B-B75261541CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="973" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="973" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="18" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="305">
   <si>
     <t>response_format_type</t>
   </si>
@@ -286,9 +286,6 @@
   </si>
   <si>
     <t>Département de la demande</t>
-  </si>
-  <si>
-    <t/>
   </si>
   <si>
     <t>78</t>
@@ -940,9 +937,6 @@
     <t>{departement} == 92</t>
   </si>
   <si>
-    <t>condition</t>
-  </si>
-  <si>
     <t>VERS, RAMB, SGEL, MLJ, ANT, BOULO, NANTER, TOTO</t>
   </si>
   <si>
@@ -968,6 +962,42 @@
   </si>
   <si>
     <t>json_object</t>
+  </si>
+  <si>
+    <t>{departeme2nt} == 78</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>True</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>condition_python</t>
+  </si>
+  <si>
+    <t>condition_javascript</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>{departement} === 78</t>
+  </si>
+  <si>
+    <t>{departement} === 92</t>
+  </si>
+  <si>
+    <t>departeme2nt: Erroneous, to check that cas is appropriately handled</t>
+  </si>
+  <si>
+    <t>{departeme2nt} === 78</t>
   </si>
 </sst>
 </file>
@@ -1004,7 +1034,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1019,12 +1049,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1096,17 +1120,17 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1416,36 +1440,36 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>133</v>
-      </c>
-      <c r="B3" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B5" s="13">
         <v>8002</v>
@@ -1462,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40884519-E9E2-4702-AA20-B46B229B9942}">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,30 +1502,30 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>14</v>
@@ -1510,15 +1534,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>51</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
@@ -1526,20 +1550,16 @@
       <c r="E6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="1">
-        <f>LEN(A6)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>52</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>17</v>
@@ -1547,20 +1567,16 @@
       <c r="E7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="1">
-        <f t="shared" ref="F7:F24" si="0">LEN(A7)</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>18</v>
@@ -1568,20 +1584,16 @@
       <c r="E8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="1">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>53</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>19</v>
@@ -1589,20 +1601,16 @@
       <c r="E9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="1">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>54</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>20</v>
@@ -1610,20 +1618,16 @@
       <c r="E10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="1">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
@@ -1631,20 +1635,16 @@
       <c r="E11" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="1">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>22</v>
@@ -1652,20 +1652,16 @@
       <c r="E12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="1">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>23</v>
@@ -1673,20 +1669,16 @@
       <c r="E13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="1">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>24</v>
@@ -1694,20 +1686,16 @@
       <c r="E14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="1">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>25</v>
@@ -1715,20 +1703,16 @@
       <c r="E15" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F15" s="1">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>26</v>
@@ -1736,20 +1720,16 @@
       <c r="E16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="1">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>27</v>
@@ -1757,20 +1737,16 @@
       <c r="E17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="1">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>28</v>
@@ -1778,20 +1754,16 @@
       <c r="E18" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="1">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>29</v>
@@ -1799,20 +1771,16 @@
       <c r="E19" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="1">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>30</v>
@@ -1820,20 +1788,16 @@
       <c r="E20" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="1">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>31</v>
@@ -1841,20 +1805,16 @@
       <c r="E21" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="F21" s="1">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>32</v>
@@ -1862,20 +1822,16 @@
       <c r="E22" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="1">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>33</v>
@@ -1883,36 +1839,22 @@
       <c r="E23" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="1">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="F24" s="1">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F25" s="1">
-        <f>MAX(F6:F24)</f>
-        <v>34</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1925,7 +1867,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1944,18 +1886,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="7" t="b">
-        <v>1</v>
+        <v>114</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -1990,10 +1932,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2006,7 +1948,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2029,25 +1971,25 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>71</v>
@@ -2056,25 +1998,25 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>97</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>98</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" s="5">
         <v>587</v>
@@ -2082,14 +2024,14 @@
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="17" t="s">
-        <v>220</v>
-      </c>
-      <c r="B8" s="5" t="b">
-        <v>0</v>
+      <c r="A8" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>296</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2106,7 +2048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -2123,50 +2065,50 @@
         <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="C1" s="9" t="s">
-        <v>164</v>
-      </c>
       <c r="D1" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>211</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>213</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>123</v>
-      </c>
       <c r="E3" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2202,30 +2144,30 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="255" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="270" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>275</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -2239,7 +2181,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549C78AA-1218-455B-9887-3E0A5E59C6C7}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -2263,68 +2205,68 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="C6" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -2349,46 +2291,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>223</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>228</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>240</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>243</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -2398,10 +2340,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A280385-38F0-446C-9432-C0DF8BDF752B}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2414,61 +2356,55 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>224</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>230</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>231</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>238</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2479,8 +2415,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2507,582 +2443,582 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>75</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="P1" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="N2" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="P2" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="Q1" s="4" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="C2" s="7" t="s">
+      <c r="Q2" s="8" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>170</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="E2" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>144</v>
-      </c>
-      <c r="K2" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="L2" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="M2" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="N2" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="O2" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q2" s="8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>171</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="E3" s="7" t="b">
-        <v>1</v>
+      <c r="E3" s="8" t="s">
+        <v>295</v>
       </c>
       <c r="F3" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="J3" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="I3" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>80</v>
-      </c>
       <c r="K3" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="L3" s="8" t="b">
-        <v>1</v>
+        <v>93</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>295</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q3" s="8" t="b">
-        <v>1</v>
+        <v>83</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="E4" s="7" t="b">
-        <v>1</v>
+      <c r="E4" s="8" t="s">
+        <v>295</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="L4" s="8" t="b">
-        <v>1</v>
+        <v>94</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>295</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="P4" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q4" s="8" t="b">
-        <v>0</v>
+        <v>83</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="E5" s="7" t="b">
-        <v>1</v>
+      <c r="E5" s="8" t="s">
+        <v>295</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="L5" s="8" t="b">
-        <v>1</v>
+        <v>94</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>295</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="P5" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q5" s="8" t="b">
-        <v>0</v>
+        <v>83</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E6" s="7" t="b">
-        <v>1</v>
+      <c r="E6" s="8" t="s">
+        <v>295</v>
       </c>
       <c r="F6" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="M6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="N6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="O6" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="P6" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q6" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="G6" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="L6" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="N6" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="O6" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q6" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="B7" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="B7" s="18" t="s">
+      <c r="G7" s="16" t="s">
+        <v>149</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="I7" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="M7" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="N7" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="O7" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q7" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C8" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>146</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="I8" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="M8" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="N8" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="O8" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="P8" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q8" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="C9" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="E7" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F7" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="G7" s="16" t="s">
-        <v>150</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="I7" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="J7" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="L7" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="M7" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="N7" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="O7" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="P7" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q7" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="B8" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>176</v>
-      </c>
-      <c r="E8" s="7" t="b">
-        <v>0</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="G8" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="K8" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="L8" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="M8" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="N8" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="O8" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="P8" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q8" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>178</v>
-      </c>
       <c r="D9" s="7" t="s">
-        <v>141</v>
-      </c>
-      <c r="E9" s="7" t="b">
-        <v>1</v>
+        <v>140</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>295</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="L9" s="8" t="b">
-        <v>1</v>
+        <v>94</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>295</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>51</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>56</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q9" s="5" t="b">
-        <v>1</v>
+        <v>84</v>
+      </c>
+      <c r="Q9" s="8" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="17" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="E10" s="7" t="b">
-        <v>1</v>
+        <v>81</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>295</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="L10" s="7" t="b">
-        <v>0</v>
+        <v>94</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>296</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>79</v>
+        <v>294</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="O10" s="7" t="s">
         <v>50</v>
       </c>
       <c r="P10" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q10" s="8" t="b">
-        <v>1</v>
+        <v>84</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="I11" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="L11" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="O11" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="B11" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>180</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>181</v>
-      </c>
-      <c r="E11" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="G11" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="I11" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="L11" s="8" t="b">
-        <v>1</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>251</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>117</v>
-      </c>
       <c r="P11" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="Q11" s="5" t="b">
-        <v>1</v>
+        <v>84</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>295</v>
       </c>
     </row>
   </sheetData>
@@ -3098,129 +3034,157 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6ECAA67-41A6-4458-95C4-500183FDE676}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>297</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B3" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D3" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="G3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
-        <v>155</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>152</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>153</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="B6" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>279</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="B7" s="7" t="s">
         <v>280</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="B8" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>283</v>
-      </c>
       <c r="C8" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>300</v>
       </c>
     </row>
   </sheetData>
@@ -3232,8 +3196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3257,19 +3221,19 @@
       <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="19" t="s">
-        <v>288</v>
-      </c>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
+      <c r="D1" s="18" t="s">
+        <v>286</v>
+      </c>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -3279,16 +3243,16 @@
         <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -3307,16 +3271,16 @@
         <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -3341,10 +3305,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -3357,22 +3321,22 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>267</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -3405,10 +3369,10 @@
     </row>
     <row r="7" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3428,7 +3392,7 @@
         <v>65</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -3445,10 +3409,10 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="B9" s="2" t="b">
-        <v>1</v>
+        <v>107</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>295</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -3465,10 +3429,10 @@
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="B10" s="2" t="b">
-        <v>1</v>
+        <v>108</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>296</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -3512,7 +3476,7 @@
         <v>64</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>66</v>
@@ -3523,10 +3487,10 @@
         <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -3534,7 +3498,7 @@
         <v>59</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>60</v>
@@ -3545,10 +3509,10 @@
         <v>61</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3556,10 +3520,10 @@
         <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3567,10 +3531,10 @@
         <v>63</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve management of dynamic list
</commit_message>
<xml_diff>
--- a/apps/delphes/runtime/configuration_delphes_ff.xlsx
+++ b/apps/delphes/runtime/configuration_delphes_ff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\apps\delphes\runtime\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7EACC30-1621-4C02-9A1B-B75261541CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D20DB57-99E1-414B-BCA9-591447643906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="973" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="973" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="common" sheetId="18" r:id="rId1"/>
@@ -27,6 +27,8 @@
     <sheet name="drools" sheetId="16" r:id="rId12"/>
     <sheet name="email_configuration" sheetId="13" r:id="rId13"/>
     <sheet name="email_templates" sheetId="11" r:id="rId14"/>
+    <sheet name="app_specific_tabs" sheetId="22" r:id="rId15"/>
+    <sheet name="arrondissements" sheetId="23" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="536" uniqueCount="307">
   <si>
     <t>response_format_type</t>
   </si>
@@ -482,9 +484,6 @@
     <t>Date d'expiration de l'API au format JJ/MM/AAAA</t>
   </si>
   <si>
-    <t>allowed_values_csv</t>
-  </si>
-  <si>
     <t>DD/MM/YYYY</t>
   </si>
   <si>
@@ -937,9 +936,6 @@
     <t>{departement} == 92</t>
   </si>
   <si>
-    <t>VERS, RAMB, SGEL, MLJ, ANT, BOULO, NANTER, TOTO</t>
-  </si>
-  <si>
     <t>openai, ollama or scaleway</t>
   </si>
   <si>
@@ -967,9 +963,6 @@
     <t>{departeme2nt} == 78</t>
   </si>
   <si>
-    <t>""</t>
-  </si>
-  <si>
     <t>True</t>
   </si>
   <si>
@@ -998,6 +991,21 @@
   </si>
   <si>
     <t>{departeme2nt} === 78</t>
+  </si>
+  <si>
+    <t>arrondissements</t>
+  </si>
+  <si>
+    <t>allowed_values_list_name</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t># If an element must be always present, us 'True in condition_python and 'true in condition_javascript</t>
+  </si>
+  <si>
+    <t>departeme2nt: Erroneous, to check that that case is appropriately handled</t>
   </si>
 </sst>
 </file>
@@ -1123,14 +1131,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1443,7 +1451,7 @@
         <v>130</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -1504,12 +1512,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1522,10 +1530,10 @@
         <v>9</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>14</v>
@@ -1539,10 +1547,10 @@
         <v>51</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>16</v>
@@ -1556,10 +1564,10 @@
         <v>52</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>17</v>
@@ -1570,13 +1578,13 @@
     </row>
     <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>18</v>
@@ -1590,10 +1598,10 @@
         <v>53</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>19</v>
@@ -1607,10 +1615,10 @@
         <v>54</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>20</v>
@@ -1621,13 +1629,13 @@
     </row>
     <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>21</v>
@@ -1638,13 +1646,13 @@
     </row>
     <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>22</v>
@@ -1655,13 +1663,13 @@
     </row>
     <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>23</v>
@@ -1672,13 +1680,13 @@
     </row>
     <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>24</v>
@@ -1689,13 +1697,13 @@
     </row>
     <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>25</v>
@@ -1706,13 +1714,13 @@
     </row>
     <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>26</v>
@@ -1723,13 +1731,13 @@
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>27</v>
@@ -1740,13 +1748,13 @@
     </row>
     <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>28</v>
@@ -1757,13 +1765,13 @@
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>29</v>
@@ -1774,13 +1782,13 @@
     </row>
     <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>30</v>
@@ -1791,13 +1799,13 @@
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>31</v>
@@ -1808,13 +1816,13 @@
     </row>
     <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>32</v>
@@ -1825,13 +1833,13 @@
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>33</v>
@@ -1842,19 +1850,19 @@
     </row>
     <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>34</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -1897,7 +1905,7 @@
         <v>114</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2025,13 +2033,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
@@ -2048,8 +2056,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2065,10 +2073,10 @@
         <v>9</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>162</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>163</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>91</v>
@@ -2082,10 +2090,10 @@
         <v>117</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>90</v>
@@ -2099,16 +2107,198 @@
         <v>121</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>212</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>122</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>124</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F8AFBFA-5790-4484-BB1A-96526826C9C1}">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z35" sqref="Z35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{316FA168-2252-420B-B68F-E9525D61AA2D}">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L13" sqref="L13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="G5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>299</v>
       </c>
     </row>
   </sheetData>
@@ -2155,19 +2345,19 @@
     </row>
     <row r="3" spans="1:3" ht="255" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="270" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>273</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>274</v>
       </c>
       <c r="C4" s="5"/>
     </row>
@@ -2205,37 +2395,37 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -2255,10 +2445,10 @@
         <v>110</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>270</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2291,46 +2481,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>222</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>225</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>239</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>242</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -2356,53 +2546,53 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>222</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>223</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>230</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>237</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -2415,9 +2605,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2427,7 +2615,7 @@
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="48.5703125" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.42578125" customWidth="1"/>
     <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.140625" customWidth="1"/>
     <col min="12" max="12" width="11.140625" customWidth="1"/>
@@ -2446,25 +2634,25 @@
         <v>136</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>137</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>141</v>
+        <v>303</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>75</v>
@@ -2479,7 +2667,7 @@
         <v>80</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>15</v>
@@ -2499,49 +2687,49 @@
         <v>138</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>139</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="H2" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>304</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>142</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>143</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>93</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>83</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -2552,25 +2740,25 @@
         <v>10</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>78</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>79</v>
@@ -2579,22 +2767,22 @@
         <v>93</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="P3" s="7" t="s">
         <v>83</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -2605,25 +2793,25 @@
         <v>10</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>70</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>87</v>
@@ -2632,22 +2820,22 @@
         <v>94</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="P4" s="7" t="s">
         <v>83</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -2658,25 +2846,25 @@
         <v>10</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>68</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>88</v>
@@ -2685,22 +2873,22 @@
         <v>94</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="P5" s="7" t="s">
         <v>83</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -2711,25 +2899,25 @@
         <v>10</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>73</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>100</v>
@@ -2738,75 +2926,75 @@
         <v>94</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="P6" s="7" t="s">
         <v>83</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>284</v>
+        <v>302</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K7" s="11" t="s">
         <v>94</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="P7" s="7" t="s">
         <v>83</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -2817,25 +3005,25 @@
         <v>10</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>174</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>175</v>
-      </c>
       <c r="E8" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>106</v>
@@ -2844,22 +3032,22 @@
         <v>94</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="P8" s="7" t="s">
         <v>83</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -2870,40 +3058,40 @@
         <v>138</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>140</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="K9" s="8" t="s">
         <v>94</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>51</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>56</v>
@@ -2912,7 +3100,7 @@
         <v>84</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -2923,40 +3111,40 @@
         <v>11</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>81</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>94</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O10" s="7" t="s">
         <v>50</v>
@@ -2965,7 +3153,7 @@
         <v>84</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -2976,40 +3164,40 @@
         <v>11</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>180</v>
-      </c>
       <c r="E11" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>294</v>
+        <v>304</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>94</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>116</v>
@@ -3018,7 +3206,7 @@
         <v>84</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -3037,7 +3225,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3053,138 +3241,138 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="G3" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>157</v>
-      </c>
       <c r="C5" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>278</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>280</v>
-      </c>
       <c r="C7" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>282</v>
-      </c>
       <c r="C8" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -3221,19 +3409,19 @@
       <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>286</v>
-      </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
+      <c r="D1" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -3243,16 +3431,16 @@
         <v>13</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -3271,16 +3459,16 @@
         <v>8</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -3305,10 +3493,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -3321,22 +3509,22 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>266</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -3369,10 +3557,10 @@
     </row>
     <row r="7" spans="1:14" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3392,7 +3580,7 @@
         <v>65</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -3411,8 +3599,8 @@
       <c r="A9" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B9" s="20" t="s">
-        <v>295</v>
+      <c r="B9" s="18" t="s">
+        <v>292</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
@@ -3431,8 +3619,8 @@
       <c r="A10" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>296</v>
+      <c r="B10" s="18" t="s">
+        <v>293</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
@@ -3476,7 +3664,7 @@
         <v>64</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>66</v>
@@ -3487,10 +3675,10 @@
         <v>58</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -3498,7 +3686,7 @@
         <v>59</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>60</v>
@@ -3509,10 +3697,10 @@
         <v>61</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -3520,10 +3708,10 @@
         <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -3531,10 +3719,10 @@
         <v>63</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>

</xml_diff>